<commit_message>
final updates after first optimization- all good to go for next optimization
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sejaldua/Desktop/DIS/AI/sejelo-searchclient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC264F03-F293-E145-9E4A-3A7C9B892D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F7D6E6-ADD0-384E-8732-F8418FB5D993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="12260" windowHeight="16820" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="17">
   <si>
     <t>Level</t>
   </si>
@@ -69,9 +69,6 @@
     <t>SACrunch</t>
   </si>
   <si>
-    <t>Table 2: Benchmarks for Exercises 1 and 2</t>
-  </si>
-  <si>
     <t>Time (s)</t>
   </si>
   <si>
@@ -81,10 +78,10 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>SAD2*</t>
-  </si>
-  <si>
-    <t>* = may have been optimized when we ran it</t>
+    <t>Table 1: Benchmarks for Exercise 1</t>
+  </si>
+  <si>
+    <t>Table 2: Optimized Implementation #1 of Exercise 2</t>
   </si>
 </sst>
 </file>
@@ -641,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7093C41-8786-554E-A962-A4525C17734E}">
-  <dimension ref="B1:H18"/>
+  <dimension ref="B1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,7 +658,7 @@
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -678,10 +675,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>2</v>
@@ -698,10 +695,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="9">
-        <v>0.121</v>
+        <v>0.151</v>
       </c>
       <c r="E4" s="9">
-        <v>12.93</v>
+        <v>25.28</v>
       </c>
       <c r="F4" s="9">
         <v>19</v>
@@ -718,10 +715,10 @@
         <v>6</v>
       </c>
       <c r="D5" s="10">
-        <v>0.125</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="E5" s="10">
-        <v>14.02</v>
+        <v>15.02</v>
       </c>
       <c r="F5" s="10">
         <v>27</v>
@@ -738,13 +735,13 @@
         <v>5</v>
       </c>
       <c r="D6" s="9">
-        <v>9.9930000000000003</v>
+        <v>67.546999999999997</v>
       </c>
       <c r="E6" s="9">
-        <v>1689.72</v>
+        <v>8192</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="12">
         <v>18195</v>
@@ -752,16 +749,16 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="13" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="10">
-        <v>7.9000000000000001E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E7" s="10">
-        <v>11.39</v>
+        <v>12.39</v>
       </c>
       <c r="F7" s="10">
         <v>25</v>
@@ -778,13 +775,13 @@
         <v>5</v>
       </c>
       <c r="D8" s="9">
-        <v>15.377000000000001</v>
+        <v>58.088999999999999</v>
       </c>
       <c r="E8" s="9">
-        <v>3053.72</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>15</v>
+        <v>8122.34</v>
+      </c>
+      <c r="F8" s="9">
+        <v>8</v>
       </c>
       <c r="G8" s="12">
         <v>30799</v>
@@ -798,10 +795,10 @@
         <v>6</v>
       </c>
       <c r="D9" s="10">
-        <v>0.158</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="E9" s="10">
-        <v>32.35</v>
+        <v>36.94</v>
       </c>
       <c r="F9" s="10">
         <v>60</v>
@@ -818,10 +815,10 @@
         <v>5</v>
       </c>
       <c r="D10" s="9">
-        <v>0.58499999999999996</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="E10" s="9">
-        <v>139.22</v>
+        <v>135.57</v>
       </c>
       <c r="F10" s="9">
         <v>3</v>
@@ -838,13 +835,13 @@
         <v>6</v>
       </c>
       <c r="D11" s="10">
-        <v>6.8769999999999998</v>
+        <v>24.14</v>
       </c>
       <c r="E11" s="10">
-        <v>1204.28</v>
+        <v>8192</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="14">
         <v>30012</v>
@@ -857,10 +854,18 @@
       <c r="C12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="12"/>
+      <c r="D12" s="9">
+        <v>27.82</v>
+      </c>
+      <c r="E12" s="9">
+        <v>8192</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="12">
+        <v>81629</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
@@ -870,16 +875,16 @@
         <v>6</v>
       </c>
       <c r="D13" s="10">
-        <v>17.640999999999998</v>
+        <v>24.06</v>
       </c>
       <c r="E13" s="10">
-        <v>4027.26</v>
+        <v>8192</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" s="14">
-        <v>44618</v>
+        <v>87730</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
@@ -890,16 +895,16 @@
         <v>5</v>
       </c>
       <c r="D14" s="9">
-        <v>13.548999999999999</v>
+        <v>34.701000000000001</v>
       </c>
       <c r="E14" s="9">
-        <v>3516.72</v>
+        <v>8192</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="12">
-        <v>37927</v>
+        <v>87572</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -910,26 +915,293 @@
         <v>6</v>
       </c>
       <c r="D15" s="16">
-        <v>37.097000000000001</v>
+        <v>19.646999999999998</v>
       </c>
       <c r="E15" s="16">
-        <v>7825.72</v>
+        <v>8192</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" s="17">
+        <v>73865</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="9">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E19" s="9">
+        <v>15.68</v>
+      </c>
+      <c r="F19" s="9">
+        <v>19</v>
+      </c>
+      <c r="G19" s="12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="E20" s="10">
+        <v>11.4</v>
+      </c>
+      <c r="F20" s="10">
+        <v>27</v>
+      </c>
+      <c r="G20" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="9">
+        <v>67.188999999999993</v>
+      </c>
+      <c r="E21" s="9">
+        <v>8192</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="12">
+        <v>219020</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="10">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="E22" s="10">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="F22" s="10">
+        <v>25</v>
+      </c>
+      <c r="G22" s="14">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="9">
+        <v>17.149000000000001</v>
+      </c>
+      <c r="E23" s="9">
+        <v>3307.72</v>
+      </c>
+      <c r="F23" s="9">
+        <v>8</v>
+      </c>
+      <c r="G23" s="12">
+        <v>89112</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="E24" s="10">
+        <v>15.34</v>
+      </c>
+      <c r="F24" s="10">
+        <v>60</v>
+      </c>
+      <c r="G24" s="14">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="E25" s="9">
+        <v>60.2</v>
+      </c>
+      <c r="F25" s="9">
+        <v>3</v>
+      </c>
+      <c r="G25" s="12">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="10">
+        <v>28.762</v>
+      </c>
+      <c r="E26" s="10">
+        <v>8192</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="14">
+        <v>204410</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="9">
+        <v>43.664999999999999</v>
+      </c>
+      <c r="E27" s="9">
+        <v>8192</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="12">
+        <v>221864</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="10">
+        <v>34.055999999999997</v>
+      </c>
+      <c r="E28" s="10">
+        <v>8192</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="14">
+        <v>219263</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="9">
+        <v>48.133000000000003</v>
+      </c>
+      <c r="E29" s="9">
+        <v>8192</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="12">
+        <v>225596</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="16">
+        <v>31.986000000000001</v>
+      </c>
+      <c r="E30" s="16">
+        <v>8192</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="17">
         <v>213472</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B17:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ran benchmarks for optimization2 -- error on SAfriendofDFS
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sejaldua/Desktop/DIS/AI/sejelo-searchclient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F7D6E6-ADD0-384E-8732-F8418FB5D993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5B6064-CEBD-FB41-8EBF-2FB839DBC2AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="12260" windowHeight="16820" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
+    <workbookView xWindow="1880" yWindow="600" windowWidth="15340" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="18">
   <si>
     <t>Level</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Table 2: Optimized Implementation #1 of Exercise 2</t>
+  </si>
+  <si>
+    <t>Table 3: Optimized Implementation #2 of Exercise 2</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -223,17 +226,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -244,7 +240,31 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -252,8 +272,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -261,7 +285,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -282,34 +308,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -322,6 +336,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -638,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7093C41-8786-554E-A962-A4525C17734E}">
-  <dimension ref="B1:H30"/>
+  <dimension ref="B1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:G17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,18 +683,18 @@
   <sheetData>
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -683,263 +709,263 @@
       <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
         <v>0.151</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>25.28</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="6">
         <v>19</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="9">
         <v>80</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="7">
         <v>15.02</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>27</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="11">
         <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6">
         <v>67.546999999999997</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>8192</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="9">
         <v>18195</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="7">
         <v>12.39</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>25</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="11">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="9">
+      <c r="C8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6">
         <v>58.088999999999999</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="6">
         <v>8122.34</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="6">
         <v>8</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="9">
         <v>30799</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="C9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7">
         <v>0.17100000000000001</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="7">
         <v>36.94</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="7">
         <v>60</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="11">
         <v>305</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="C10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6">
         <v>0.45500000000000002</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="6">
         <v>135.57</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="6">
         <v>3</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="9">
         <v>1227</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="10">
+      <c r="C11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="7">
         <v>24.14</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="7">
         <v>8192</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="11">
         <v>30012</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="9">
+      <c r="C12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6">
         <v>27.82</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="6">
         <v>8192</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="9">
         <v>81629</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="10">
+      <c r="C13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="7">
         <v>24.06</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="7">
         <v>8192</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="11">
         <v>87730</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="9">
+      <c r="C14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6">
         <v>34.701000000000001</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="6">
         <v>8192</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="9">
         <v>87572</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="16">
+      <c r="C15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="13">
         <v>19.646999999999998</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="13">
         <v>8192</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="14">
         <v>73865</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -954,255 +980,512 @@
       <c r="F18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="9">
+      <c r="C19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="6">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="6">
         <v>15.68</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="6">
         <v>19</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="9">
         <v>80</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="10">
+      <c r="C20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="7">
         <v>0.13</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="7">
         <v>11.4</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="7">
         <v>27</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="11">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="9">
+      <c r="C21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="6">
         <v>67.188999999999993</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="6">
         <v>8192</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="9">
         <v>219020</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="10">
+      <c r="C22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="7">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="7">
         <v>9.1199999999999992</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="7">
         <v>25</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="11">
         <v>86</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="9">
+      <c r="C23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6">
         <v>17.149000000000001</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="6">
         <v>3307.72</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="6">
         <v>8</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="9">
         <v>89112</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="10">
+      <c r="C24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="7">
         <v>0.10100000000000001</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="7">
         <v>15.34</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="7">
         <v>60</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="11">
         <v>305</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="9">
+      <c r="C25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="6">
         <v>60.2</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="6">
         <v>3</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="9">
         <v>1227</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="10">
+      <c r="C26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="7">
         <v>28.762</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="7">
         <v>8192</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="11">
         <v>204410</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="9">
+      <c r="C27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6">
         <v>43.664999999999999</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="6">
         <v>8192</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="9">
         <v>221864</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="10">
+      <c r="C28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="7">
         <v>34.055999999999997</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="7">
         <v>8192</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="11">
         <v>219263</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="9">
+      <c r="C29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6">
         <v>48.133000000000003</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="6">
         <v>8192</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="9">
         <v>225596</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="16">
+      <c r="C30" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="13">
         <v>31.986000000000001</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="13">
         <v>8192</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="17">
+      <c r="G30" s="14">
         <v>213472</v>
       </c>
     </row>
+    <row r="31" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="6">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E34" s="6">
+        <v>3.72</v>
+      </c>
+      <c r="F34" s="6">
+        <v>19</v>
+      </c>
+      <c r="G34" s="9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E35" s="7">
+        <v>3.59</v>
+      </c>
+      <c r="F35" s="7">
+        <v>27</v>
+      </c>
+      <c r="G35" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="6">
+        <v>14.467000000000001</v>
+      </c>
+      <c r="E36" s="6">
+        <v>692.72</v>
+      </c>
+      <c r="F36" s="6">
+        <v>19</v>
+      </c>
+      <c r="G36" s="9">
+        <v>635190</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="7">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E37" s="7">
+        <v>3.59</v>
+      </c>
+      <c r="F37" s="7">
+        <v>25</v>
+      </c>
+      <c r="G37" s="11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="9"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B40" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="6">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E40" s="6">
+        <v>5.12</v>
+      </c>
+      <c r="F40" s="6">
+        <v>3</v>
+      </c>
+      <c r="G40" s="9">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="7">
+        <v>35.552</v>
+      </c>
+      <c r="E41" s="7">
+        <v>2015.72</v>
+      </c>
+      <c r="F41" s="7">
+        <v>981528</v>
+      </c>
+      <c r="G41" s="11">
+        <v>2953986</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B42" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="6">
+        <v>18.260999999999999</v>
+      </c>
+      <c r="E42" s="6">
+        <v>2252.7199999999998</v>
+      </c>
+      <c r="F42" s="6">
+        <v>60</v>
+      </c>
+      <c r="G42" s="6">
+        <v>1961416</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B43" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="7">
+        <v>24.539000000000001</v>
+      </c>
+      <c r="E43" s="7">
+        <v>4101.72</v>
+      </c>
+      <c r="F43" s="7">
+        <v>2517074</v>
+      </c>
+      <c r="G43" s="11">
+        <v>4089953</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="6">
+        <v>179.98599999999999</v>
+      </c>
+      <c r="E44" s="6">
+        <v>3840.72</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="9">
+        <v>6464388</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="13">
+        <v>9.218</v>
+      </c>
+      <c r="E45" s="13">
+        <v>4392.28</v>
+      </c>
+      <c r="F45" s="13">
+        <v>380992</v>
+      </c>
+      <c r="G45" s="14">
+        <v>1023377</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B32:G32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
exercises 3: done, exercise 4: partially done
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sejaldua/Desktop/DIS/AI/sejelo-searchclient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5B6064-CEBD-FB41-8EBF-2FB839DBC2AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCB3725-2B18-2640-9B6B-D32F19B16E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="600" windowWidth="15340" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
+    <workbookView xWindow="1880" yWindow="600" windowWidth="19260" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -664,826 +664,841 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7093C41-8786-554E-A962-A4525C17734E}">
-  <dimension ref="B1:H45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="18" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="17.5" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="15" t="s">
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>5</v>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.151</v>
       </c>
       <c r="D4" s="6">
-        <v>0.151</v>
+        <v>25.28</v>
       </c>
       <c r="E4" s="6">
-        <v>25.28</v>
-      </c>
-      <c r="F4" s="6">
         <v>19</v>
       </c>
-      <c r="G4" s="9">
+      <c r="F4" s="9">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>6</v>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.10199999999999999</v>
       </c>
       <c r="D5" s="7">
-        <v>0.10199999999999999</v>
+        <v>15.02</v>
       </c>
       <c r="E5" s="7">
-        <v>15.02</v>
-      </c>
-      <c r="F5" s="7">
         <v>27</v>
       </c>
-      <c r="G5" s="11">
+      <c r="F5" s="11">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>5</v>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>67.546999999999997</v>
       </c>
       <c r="D6" s="6">
-        <v>67.546999999999997</v>
-      </c>
-      <c r="E6" s="6">
         <v>8192</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="9">
+      <c r="F6" s="9">
         <v>18195</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>6</v>
+      <c r="B7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="D7" s="7">
-        <v>8.8999999999999996E-2</v>
+        <v>12.39</v>
       </c>
       <c r="E7" s="7">
-        <v>12.39</v>
-      </c>
-      <c r="F7" s="7">
         <v>25</v>
       </c>
-      <c r="G7" s="11">
+      <c r="F7" s="11">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>5</v>
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6">
+        <v>58.088999999999999</v>
       </c>
       <c r="D8" s="6">
-        <v>58.088999999999999</v>
+        <v>8122.34</v>
       </c>
       <c r="E8" s="6">
-        <v>8122.34</v>
-      </c>
-      <c r="F8" s="6">
         <v>8</v>
       </c>
-      <c r="G8" s="9">
+      <c r="F8" s="9">
         <v>30799</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>6</v>
+      <c r="B9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.17100000000000001</v>
       </c>
       <c r="D9" s="7">
-        <v>0.17100000000000001</v>
+        <v>36.94</v>
       </c>
       <c r="E9" s="7">
-        <v>36.94</v>
-      </c>
-      <c r="F9" s="7">
         <v>60</v>
       </c>
-      <c r="G9" s="11">
+      <c r="F9" s="11">
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>5</v>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.45500000000000002</v>
       </c>
       <c r="D10" s="6">
-        <v>0.45500000000000002</v>
+        <v>135.57</v>
       </c>
       <c r="E10" s="6">
-        <v>135.57</v>
-      </c>
-      <c r="F10" s="6">
         <v>3</v>
       </c>
-      <c r="G10" s="9">
+      <c r="F10" s="9">
         <v>1227</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>6</v>
+      <c r="B11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="7">
+        <v>24.14</v>
       </c>
       <c r="D11" s="7">
-        <v>24.14</v>
-      </c>
-      <c r="E11" s="7">
         <v>8192</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="11">
+      <c r="F11" s="11">
         <v>30012</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>5</v>
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6">
+        <v>27.82</v>
       </c>
       <c r="D12" s="6">
-        <v>27.82</v>
-      </c>
-      <c r="E12" s="6">
         <v>8192</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="9">
+      <c r="F12" s="9">
         <v>81629</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>6</v>
+      <c r="B13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7">
+        <v>24.06</v>
       </c>
       <c r="D13" s="7">
-        <v>24.06</v>
-      </c>
-      <c r="E13" s="7">
         <v>8192</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="11">
+      <c r="F13" s="11">
         <v>87730</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="8" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>5</v>
+      <c r="B14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="6">
+        <v>34.701000000000001</v>
       </c>
       <c r="D14" s="6">
-        <v>34.701000000000001</v>
-      </c>
-      <c r="E14" s="6">
         <v>8192</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="9">
+      <c r="F14" s="9">
         <v>87572</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+    <row r="15" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>6</v>
+      <c r="B15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="13">
+        <v>19.646999999999998</v>
       </c>
       <c r="D15" s="13">
-        <v>19.646999999999998</v>
-      </c>
-      <c r="E15" s="13">
         <v>8192</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="E15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="14">
+      <c r="F15" s="14">
         <v>73865</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="15" t="s">
+    <row r="16" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
         <v>16</v>
       </c>
+      <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B18" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="C18" s="3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>5</v>
+      <c r="B19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="6">
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="D19" s="6">
-        <v>8.6999999999999994E-2</v>
+        <v>15.68</v>
       </c>
       <c r="E19" s="6">
-        <v>15.68</v>
-      </c>
-      <c r="F19" s="6">
         <v>19</v>
       </c>
-      <c r="G19" s="9">
+      <c r="F19" s="9">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="10" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>6</v>
+      <c r="B20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.13</v>
       </c>
       <c r="D20" s="7">
-        <v>0.13</v>
+        <v>11.4</v>
       </c>
       <c r="E20" s="7">
-        <v>11.4</v>
-      </c>
-      <c r="F20" s="7">
         <v>27</v>
       </c>
-      <c r="G20" s="11">
+      <c r="F20" s="11">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>5</v>
+      <c r="B21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="6">
+        <v>67.188999999999993</v>
       </c>
       <c r="D21" s="6">
-        <v>67.188999999999993</v>
-      </c>
-      <c r="E21" s="6">
         <v>8192</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="9">
+      <c r="F21" s="9">
         <v>219020</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="10" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>6</v>
+      <c r="B22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="7">
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="D22" s="7">
-        <v>6.9000000000000006E-2</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="E22" s="7">
-        <v>9.1199999999999992</v>
-      </c>
-      <c r="F22" s="7">
         <v>25</v>
       </c>
-      <c r="G22" s="11">
+      <c r="F22" s="11">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="8" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>5</v>
+      <c r="B23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="6">
+        <v>17.149000000000001</v>
       </c>
       <c r="D23" s="6">
-        <v>17.149000000000001</v>
+        <v>3307.72</v>
       </c>
       <c r="E23" s="6">
-        <v>3307.72</v>
-      </c>
-      <c r="F23" s="6">
         <v>8</v>
       </c>
-      <c r="G23" s="9">
+      <c r="F23" s="9">
         <v>89112</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="10" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>6</v>
+      <c r="B24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.10100000000000001</v>
       </c>
       <c r="D24" s="7">
-        <v>0.10100000000000001</v>
+        <v>15.34</v>
       </c>
       <c r="E24" s="7">
-        <v>15.34</v>
-      </c>
-      <c r="F24" s="7">
         <v>60</v>
       </c>
-      <c r="G24" s="11">
+      <c r="F24" s="11">
         <v>305</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="8" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>5</v>
+      <c r="B25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.28799999999999998</v>
       </c>
       <c r="D25" s="6">
-        <v>0.28799999999999998</v>
+        <v>60.2</v>
       </c>
       <c r="E25" s="6">
-        <v>60.2</v>
-      </c>
-      <c r="F25" s="6">
         <v>3</v>
       </c>
-      <c r="G25" s="9">
+      <c r="F25" s="9">
         <v>1227</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="10" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>6</v>
+      <c r="B26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="7">
+        <v>28.762</v>
       </c>
       <c r="D26" s="7">
-        <v>28.762</v>
-      </c>
-      <c r="E26" s="7">
         <v>8192</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="E26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="11">
+      <c r="F26" s="11">
         <v>204410</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="8" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>5</v>
+      <c r="B27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="6">
+        <v>43.664999999999999</v>
       </c>
       <c r="D27" s="6">
-        <v>43.664999999999999</v>
-      </c>
-      <c r="E27" s="6">
         <v>8192</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="9">
+      <c r="F27" s="9">
         <v>221864</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="10" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>6</v>
+      <c r="B28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="7">
+        <v>34.055999999999997</v>
       </c>
       <c r="D28" s="7">
-        <v>34.055999999999997</v>
-      </c>
-      <c r="E28" s="7">
         <v>8192</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="11">
+      <c r="F28" s="11">
         <v>219263</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="8" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>5</v>
+      <c r="B29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="6">
+        <v>48.133000000000003</v>
       </c>
       <c r="D29" s="6">
-        <v>48.133000000000003</v>
-      </c>
-      <c r="E29" s="6">
         <v>8192</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="E29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="9">
+      <c r="F29" s="9">
         <v>225596</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
+    <row r="30" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>6</v>
+      <c r="B30" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="13">
+        <v>31.986000000000001</v>
       </c>
       <c r="D30" s="13">
-        <v>31.986000000000001</v>
-      </c>
-      <c r="E30" s="13">
         <v>8192</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="E30" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="14">
+      <c r="F30" s="14">
         <v>213472</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="15" t="s">
+    <row r="31" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
         <v>17</v>
       </c>
+      <c r="B32" s="16"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="17"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="4" t="s">
+      <c r="F32" s="17"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B33" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="C33" s="3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="8" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>5</v>
+      <c r="B34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="6">
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="D34" s="6">
-        <v>2.9000000000000001E-2</v>
+        <v>3.72</v>
       </c>
       <c r="E34" s="6">
+        <v>19</v>
+      </c>
+      <c r="F34" s="9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D35" s="7">
+        <v>3.59</v>
+      </c>
+      <c r="E35" s="7">
+        <v>27</v>
+      </c>
+      <c r="F35" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="6">
+        <v>14.467000000000001</v>
+      </c>
+      <c r="D36" s="6">
+        <v>692.72</v>
+      </c>
+      <c r="E36" s="6">
+        <v>19</v>
+      </c>
+      <c r="F36" s="9">
+        <v>635190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D37" s="7">
+        <v>3.59</v>
+      </c>
+      <c r="E37" s="7">
+        <v>25</v>
+      </c>
+      <c r="F37" s="11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1.1850000000000001</v>
+      </c>
+      <c r="D38" s="6">
+        <v>72.13</v>
+      </c>
+      <c r="E38" s="6">
+        <v>8</v>
+      </c>
+      <c r="F38" s="9">
+        <v>89112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="7">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D39" s="7">
         <v>3.72</v>
       </c>
-      <c r="F34" s="6">
-        <v>19</v>
-      </c>
-      <c r="G34" s="9">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="7">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E35" s="7">
-        <v>3.59</v>
-      </c>
-      <c r="F35" s="7">
-        <v>27</v>
-      </c>
-      <c r="G35" s="11">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="6">
-        <v>14.467000000000001</v>
-      </c>
-      <c r="E36" s="6">
-        <v>692.72</v>
-      </c>
-      <c r="F36" s="6">
-        <v>19</v>
-      </c>
-      <c r="G36" s="9">
-        <v>635190</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="7">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="E37" s="7">
-        <v>3.59</v>
-      </c>
-      <c r="F37" s="7">
-        <v>25</v>
-      </c>
-      <c r="G37" s="11">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="9"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="11"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="8" t="s">
+      <c r="E39" s="7">
+        <v>60</v>
+      </c>
+      <c r="F39" s="11">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>5</v>
+      <c r="B40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="6">
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D40" s="6">
-        <v>4.8000000000000001E-2</v>
+        <v>5.12</v>
       </c>
       <c r="E40" s="6">
-        <v>5.12</v>
-      </c>
-      <c r="F40" s="6">
         <v>3</v>
       </c>
-      <c r="G40" s="9">
+      <c r="F40" s="9">
         <v>1227</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="10" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>6</v>
+      <c r="B41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="7">
+        <v>35.552</v>
       </c>
       <c r="D41" s="7">
-        <v>35.552</v>
+        <v>2015.72</v>
       </c>
       <c r="E41" s="7">
-        <v>2015.72</v>
-      </c>
-      <c r="F41" s="7">
         <v>981528</v>
       </c>
-      <c r="G41" s="11">
+      <c r="F41" s="11">
         <v>2953986</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="8" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>5</v>
+      <c r="B42" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="6">
+        <v>18.260999999999999</v>
       </c>
       <c r="D42" s="6">
-        <v>18.260999999999999</v>
+        <v>2252.7199999999998</v>
       </c>
       <c r="E42" s="6">
-        <v>2252.7199999999998</v>
+        <v>60</v>
       </c>
       <c r="F42" s="6">
-        <v>60</v>
-      </c>
-      <c r="G42" s="6">
         <v>1961416</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B43" s="10" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>6</v>
+      <c r="B43" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="7">
+        <v>24.539000000000001</v>
       </c>
       <c r="D43" s="7">
-        <v>24.539000000000001</v>
+        <v>4101.72</v>
       </c>
       <c r="E43" s="7">
-        <v>4101.72</v>
-      </c>
-      <c r="F43" s="7">
         <v>2517074</v>
       </c>
-      <c r="G43" s="11">
+      <c r="F43" s="11">
         <v>4089953</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B44" s="8" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>5</v>
+      <c r="B44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="6">
+        <v>179.98599999999999</v>
       </c>
       <c r="D44" s="6">
-        <v>179.98599999999999</v>
-      </c>
-      <c r="E44" s="6">
         <v>3840.72</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G44" s="9">
+      <c r="F44" s="9">
         <v>6464388</v>
       </c>
     </row>
-    <row r="45" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="12" t="s">
+    <row r="45" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="13" t="s">
-        <v>6</v>
+      <c r="B45" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="13">
+        <v>9.218</v>
       </c>
       <c r="D45" s="13">
-        <v>9.218</v>
+        <v>4392.28</v>
       </c>
       <c r="E45" s="13">
-        <v>4392.28</v>
-      </c>
-      <c r="F45" s="13">
         <v>380992</v>
       </c>
-      <c r="G45" s="14">
+      <c r="F45" s="14">
         <v>1023377</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Exercise 4: complete - 12 total levels created
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sejaldua/Desktop/DIS/AI/sejelo-searchclient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58D8895-7FF9-A249-A87A-FB3977C33569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004BBE42-8160-494D-A393-EAC9894C9031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="600" windowWidth="21020" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
+    <workbookView xWindow="1880" yWindow="600" windowWidth="20000" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="43">
   <si>
     <t>Level</t>
   </si>
@@ -112,6 +112,54 @@
   </si>
   <si>
     <t>Samicromouse...</t>
+  </si>
+  <si>
+    <t>SAsokoban01</t>
+  </si>
+  <si>
+    <t>SAsokoban02</t>
+  </si>
+  <si>
+    <t>SAsokoban03</t>
+  </si>
+  <si>
+    <t>SAsokoban04</t>
+  </si>
+  <si>
+    <t>SAsokoban05</t>
+  </si>
+  <si>
+    <t>SAsokoban35</t>
+  </si>
+  <si>
+    <t>SAsokoban36</t>
+  </si>
+  <si>
+    <t>SAsokoban37</t>
+  </si>
+  <si>
+    <t>SAsokoban38</t>
+  </si>
+  <si>
+    <t>SAsokoban39</t>
+  </si>
+  <si>
+    <t>SAsokoban70</t>
+  </si>
+  <si>
+    <t>SAsokoban71</t>
+  </si>
+  <si>
+    <t>SAsokoban72</t>
+  </si>
+  <si>
+    <t>SAsokoban73</t>
+  </si>
+  <si>
+    <t>SAsokoban74</t>
+  </si>
+  <si>
+    <t>Table 6: Benchmarks for Sokoban Levels - Exercise 4</t>
   </si>
 </sst>
 </file>
@@ -143,7 +191,7 @@
       <name val="Calibri Light (Body)"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,24 +212,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFCE4D6"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4DAE1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFDCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4F3FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="36">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -610,11 +682,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -678,6 +776,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -708,21 +809,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -768,22 +854,103 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -792,6 +959,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE4F3FF"/>
+      <color rgb="FFDFDCFF"/>
+      <color rgb="FFE4DAE1"/>
+      <color rgb="FFFFD0B3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1100,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7093C41-8786-554E-A962-A4525C17734E}">
-  <dimension ref="B1:H84"/>
+  <dimension ref="B1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1963,422 +2138,422 @@
       </c>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C49" s="35">
         <v>4</v>
       </c>
-      <c r="D49" s="25">
+      <c r="D49" s="36">
         <v>1.6E-2</v>
       </c>
-      <c r="E49" s="26">
+      <c r="E49" s="37">
         <v>3.59</v>
       </c>
-      <c r="F49" s="26">
+      <c r="F49" s="37">
         <v>2</v>
       </c>
-      <c r="G49" s="27">
+      <c r="G49" s="38">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="29">
+      <c r="C50" s="40">
         <v>8</v>
       </c>
-      <c r="D50" s="30">
+      <c r="D50" s="41">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E50" s="31">
+      <c r="E50" s="42">
         <v>3.59</v>
       </c>
-      <c r="F50" s="31">
+      <c r="F50" s="42">
         <v>6</v>
       </c>
-      <c r="G50" s="32">
+      <c r="G50" s="43">
         <v>15</v>
       </c>
     </row>
     <row r="51" spans="2:7">
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="29">
+      <c r="C51" s="40">
         <v>16</v>
       </c>
-      <c r="D51" s="30">
+      <c r="D51" s="41">
         <v>2.4E-2</v>
       </c>
-      <c r="E51" s="31">
+      <c r="E51" s="42">
         <v>3.59</v>
       </c>
-      <c r="F51" s="31">
+      <c r="F51" s="42">
         <v>14</v>
       </c>
-      <c r="G51" s="32">
+      <c r="G51" s="43">
         <v>68</v>
       </c>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="29">
+      <c r="C52" s="40">
         <v>32</v>
       </c>
-      <c r="D52" s="30">
+      <c r="D52" s="41">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E52" s="31">
+      <c r="E52" s="42">
         <v>4</v>
       </c>
-      <c r="F52" s="31">
+      <c r="F52" s="42">
         <v>30</v>
       </c>
-      <c r="G52" s="32">
+      <c r="G52" s="43">
         <v>266</v>
       </c>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="29">
+      <c r="C53" s="40">
         <v>64</v>
       </c>
-      <c r="D53" s="30">
+      <c r="D53" s="41">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E53" s="31">
+      <c r="E53" s="42">
         <v>6.28</v>
       </c>
-      <c r="F53" s="31">
+      <c r="F53" s="42">
         <v>62</v>
       </c>
-      <c r="G53" s="32">
+      <c r="G53" s="43">
         <v>1034</v>
       </c>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="33" t="s">
+      <c r="B54" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="34">
+      <c r="C54" s="45">
         <v>128</v>
       </c>
-      <c r="D54" s="35">
+      <c r="D54" s="46">
         <v>0.15</v>
       </c>
-      <c r="E54" s="36">
+      <c r="E54" s="47">
         <v>10.09</v>
       </c>
-      <c r="F54" s="36">
+      <c r="F54" s="47">
         <v>126</v>
       </c>
-      <c r="G54" s="37">
+      <c r="G54" s="48">
         <v>4128</v>
       </c>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="38" t="s">
+      <c r="B55" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="39">
+      <c r="C55" s="25">
         <v>4</v>
       </c>
-      <c r="D55" s="40">
+      <c r="D55" s="26">
         <v>1.9E-2</v>
       </c>
-      <c r="E55" s="41">
+      <c r="E55" s="27">
         <v>3.59</v>
       </c>
-      <c r="F55" s="41">
+      <c r="F55" s="27">
         <v>2</v>
       </c>
-      <c r="G55" s="42">
+      <c r="G55" s="28">
         <v>44</v>
       </c>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="44">
+      <c r="C56" s="30">
         <v>8</v>
       </c>
-      <c r="D56" s="45">
+      <c r="D56" s="31">
         <v>4.7E-2</v>
       </c>
-      <c r="E56" s="46">
+      <c r="E56" s="32">
         <v>5.4</v>
       </c>
-      <c r="F56" s="46">
+      <c r="F56" s="32">
         <v>6</v>
       </c>
-      <c r="G56" s="47">
+      <c r="G56" s="33">
         <v>660</v>
       </c>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="43" t="s">
+      <c r="B57" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="44">
+      <c r="C57" s="30">
         <v>16</v>
       </c>
-      <c r="D57" s="45">
+      <c r="D57" s="31">
         <v>0.32900000000000001</v>
       </c>
-      <c r="E57" s="46">
+      <c r="E57" s="32">
         <v>21.27</v>
       </c>
-      <c r="F57" s="46">
+      <c r="F57" s="32">
         <v>14</v>
       </c>
-      <c r="G57" s="47">
+      <c r="G57" s="33">
         <v>8580</v>
       </c>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="43" t="s">
+      <c r="B58" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="44">
+      <c r="C58" s="30">
         <v>32</v>
       </c>
-      <c r="D58" s="45">
+      <c r="D58" s="31">
         <v>3.6859999999999999</v>
       </c>
-      <c r="E58" s="46">
+      <c r="E58" s="32">
         <v>515.72</v>
       </c>
-      <c r="F58" s="46">
+      <c r="F58" s="32">
         <v>30</v>
       </c>
-      <c r="G58" s="47">
+      <c r="G58" s="33">
         <v>118093</v>
       </c>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="43" t="s">
+      <c r="B59" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="44">
+      <c r="C59" s="50">
         <v>64</v>
       </c>
-      <c r="D59" s="45">
+      <c r="D59" s="51">
         <v>98.825000000000003</v>
       </c>
-      <c r="E59" s="46">
+      <c r="E59" s="52">
         <v>8192</v>
       </c>
-      <c r="F59" s="46" t="s">
+      <c r="F59" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G59" s="47">
+      <c r="G59" s="53">
         <v>808491</v>
       </c>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="48" t="s">
+      <c r="B60" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="49">
+      <c r="C60" s="60">
         <v>128</v>
       </c>
-      <c r="D60" s="50">
+      <c r="D60" s="61">
         <v>65.835999999999999</v>
       </c>
-      <c r="E60" s="51">
+      <c r="E60" s="62">
         <v>8192</v>
       </c>
-      <c r="F60" s="51" t="s">
+      <c r="F60" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="G60" s="52">
+      <c r="G60" s="63">
         <v>221993</v>
       </c>
     </row>
     <row r="61" spans="2:7">
-      <c r="B61" s="28" t="s">
+      <c r="B61" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C61" s="29">
+      <c r="C61" s="40">
         <v>4</v>
       </c>
-      <c r="D61" s="30">
+      <c r="D61" s="41">
         <v>0.42899999999999999</v>
       </c>
-      <c r="E61" s="31">
+      <c r="E61" s="42">
         <v>11.63</v>
       </c>
-      <c r="F61" s="31">
+      <c r="F61" s="42">
         <v>8</v>
       </c>
-      <c r="G61" s="32">
+      <c r="G61" s="43">
         <v>17016</v>
       </c>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C62" s="29">
-        <v>5</v>
-      </c>
-      <c r="D62" s="30">
+      <c r="C62" s="40">
+        <v>5</v>
+      </c>
+      <c r="D62" s="41">
         <v>60.161000000000001</v>
       </c>
-      <c r="E62" s="31">
+      <c r="E62" s="42">
         <v>820.72</v>
       </c>
-      <c r="F62" s="31">
+      <c r="F62" s="42">
         <v>15</v>
       </c>
-      <c r="G62" s="32">
+      <c r="G62" s="43">
         <v>874805</v>
       </c>
     </row>
     <row r="63" spans="2:7">
-      <c r="B63" s="28" t="s">
+      <c r="B63" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C63" s="29">
+      <c r="C63" s="50">
         <v>6</v>
       </c>
-      <c r="D63" s="30">
+      <c r="D63" s="51">
         <v>178.28</v>
       </c>
-      <c r="E63" s="31">
+      <c r="E63" s="52">
         <v>1900.72</v>
       </c>
-      <c r="F63" s="31" t="s">
+      <c r="F63" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G63" s="32">
+      <c r="G63" s="53">
         <v>3287110</v>
       </c>
     </row>
     <row r="64" spans="2:7">
-      <c r="B64" s="28" t="s">
+      <c r="B64" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C64" s="29">
+      <c r="C64" s="50">
         <v>7</v>
       </c>
-      <c r="D64" s="30">
+      <c r="D64" s="51">
         <v>178.01</v>
       </c>
-      <c r="E64" s="31">
+      <c r="E64" s="52">
         <v>2834.72</v>
       </c>
-      <c r="F64" s="31" t="s">
+      <c r="F64" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G64" s="31">
+      <c r="G64" s="52">
         <v>4032039</v>
       </c>
     </row>
     <row r="65" spans="2:7">
-      <c r="B65" s="28" t="s">
+      <c r="B65" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C65" s="29">
+      <c r="C65" s="50">
         <v>8</v>
       </c>
-      <c r="D65" s="30">
+      <c r="D65" s="51">
         <v>179.13</v>
       </c>
-      <c r="E65" s="31">
+      <c r="E65" s="52">
         <v>3482.72</v>
       </c>
-      <c r="F65" s="31" t="s">
+      <c r="F65" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="32">
+      <c r="G65" s="53">
         <v>4734372</v>
       </c>
     </row>
     <row r="66" spans="2:7">
-      <c r="B66" s="28" t="s">
+      <c r="B66" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="29">
+      <c r="C66" s="50">
         <v>16</v>
       </c>
-      <c r="D66" s="30">
+      <c r="D66" s="51">
         <v>178.7</v>
       </c>
-      <c r="E66" s="31">
+      <c r="E66" s="52">
         <v>6819.72</v>
       </c>
-      <c r="F66" s="31" t="s">
+      <c r="F66" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G66" s="32">
+      <c r="G66" s="53">
         <v>5173127</v>
       </c>
     </row>
     <row r="67" spans="2:7">
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C67" s="29">
+      <c r="C67" s="50">
         <v>32</v>
       </c>
-      <c r="D67" s="30">
+      <c r="D67" s="51">
         <v>93.528000000000006</v>
       </c>
-      <c r="E67" s="31">
+      <c r="E67" s="52">
         <v>8192</v>
       </c>
-      <c r="F67" s="31" t="s">
+      <c r="F67" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G67" s="32">
+      <c r="G67" s="53">
         <v>2506572</v>
       </c>
     </row>
     <row r="68" spans="2:7">
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C68" s="29">
+      <c r="C68" s="50">
         <v>64</v>
       </c>
-      <c r="D68" s="30">
+      <c r="D68" s="51">
         <v>57.46</v>
       </c>
-      <c r="E68" s="31">
+      <c r="E68" s="52">
         <v>8192</v>
       </c>
-      <c r="F68" s="31" t="s">
+      <c r="F68" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G68" s="32">
+      <c r="G68" s="53">
         <v>810381</v>
       </c>
     </row>
     <row r="69" spans="2:7" ht="20" thickBot="1">
-      <c r="B69" s="53" t="s">
+      <c r="B69" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C69" s="54">
+      <c r="C69" s="55">
         <v>128</v>
       </c>
-      <c r="D69" s="55">
+      <c r="D69" s="56">
         <v>35.396999999999998</v>
       </c>
-      <c r="E69" s="56">
+      <c r="E69" s="57">
         <v>8192</v>
       </c>
-      <c r="F69" s="56" t="s">
+      <c r="F69" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G69" s="57">
+      <c r="G69" s="58">
         <v>224619</v>
       </c>
     </row>
@@ -2533,56 +2708,355 @@
         <v>396</v>
       </c>
     </row>
-    <row r="79" spans="2:7">
-      <c r="B79" s="58"/>
-      <c r="C79" s="58"/>
-      <c r="D79" s="58"/>
-      <c r="E79" s="58"/>
-      <c r="F79" s="58"/>
-      <c r="G79" s="58"/>
+    <row r="79" spans="2:7" ht="20" thickBot="1">
+      <c r="B79" s="23"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="23"/>
+      <c r="G79" s="23"/>
     </row>
     <row r="80" spans="2:7">
-      <c r="B80" s="58"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="58"/>
-      <c r="E80" s="58"/>
-      <c r="F80" s="58"/>
-      <c r="G80" s="58"/>
+      <c r="B80" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="73"/>
     </row>
     <row r="81" spans="2:7">
-      <c r="B81" s="58"/>
-      <c r="C81" s="58"/>
-      <c r="D81" s="58"/>
-      <c r="E81" s="58"/>
-      <c r="F81" s="58"/>
-      <c r="G81" s="58"/>
+      <c r="B81" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="82" spans="2:7">
-      <c r="B82" s="58"/>
-      <c r="C82" s="58"/>
-      <c r="D82" s="58"/>
-      <c r="E82" s="58"/>
-      <c r="F82" s="58"/>
-      <c r="G82" s="58"/>
+      <c r="B82" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C82" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="67">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="E82" s="68">
+        <v>5.12</v>
+      </c>
+      <c r="F82" s="68">
+        <v>34</v>
+      </c>
+      <c r="G82" s="75">
+        <v>749</v>
+      </c>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" s="58"/>
-      <c r="C83" s="58"/>
-      <c r="D83" s="58"/>
-      <c r="E83" s="58"/>
-      <c r="F83" s="58"/>
-      <c r="G83" s="58"/>
+      <c r="B83" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="C83" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="67">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="E83" s="68">
+        <v>7.68</v>
+      </c>
+      <c r="F83" s="68">
+        <v>23</v>
+      </c>
+      <c r="G83" s="75">
+        <v>1983</v>
+      </c>
     </row>
     <row r="84" spans="2:7">
-      <c r="B84" s="58"/>
-      <c r="C84" s="58"/>
-      <c r="D84" s="58"/>
-      <c r="E84" s="58"/>
-      <c r="F84" s="58"/>
-      <c r="G84" s="58"/>
+      <c r="B84" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="67">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="E84" s="68">
+        <v>10.28</v>
+      </c>
+      <c r="F84" s="68">
+        <v>31</v>
+      </c>
+      <c r="G84" s="75">
+        <v>2960</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7">
+      <c r="B85" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="67">
+        <v>0.253</v>
+      </c>
+      <c r="E85" s="68">
+        <v>21.74</v>
+      </c>
+      <c r="F85" s="68">
+        <v>25</v>
+      </c>
+      <c r="G85" s="75">
+        <v>12520</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7">
+      <c r="B86" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="C86" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="67">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="E86" s="68">
+        <v>29.66</v>
+      </c>
+      <c r="F86" s="68">
+        <v>37</v>
+      </c>
+      <c r="G86" s="75">
+        <v>22718</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7">
+      <c r="B87" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="66">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="E87" s="69">
+        <v>10.35</v>
+      </c>
+      <c r="F87" s="69">
+        <v>53</v>
+      </c>
+      <c r="G87" s="77">
+        <v>8061</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7">
+      <c r="B88" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" s="66">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="E88" s="69">
+        <v>24.18</v>
+      </c>
+      <c r="F88" s="69">
+        <v>59</v>
+      </c>
+      <c r="G88" s="77">
+        <v>18041</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7">
+      <c r="B89" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="66">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="E89" s="69">
+        <v>29.24</v>
+      </c>
+      <c r="F89" s="69">
+        <v>53</v>
+      </c>
+      <c r="G89" s="77">
+        <v>40349</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7">
+      <c r="B90" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="C90" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="66">
+        <v>0.184</v>
+      </c>
+      <c r="E90" s="69">
+        <v>7.21</v>
+      </c>
+      <c r="F90" s="69">
+        <v>75</v>
+      </c>
+      <c r="G90" s="77">
+        <v>6358</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7">
+      <c r="B91" s="76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="66">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="E91" s="69">
+        <v>12.54</v>
+      </c>
+      <c r="F91" s="69">
+        <v>60</v>
+      </c>
+      <c r="G91" s="77">
+        <v>7817</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7">
+      <c r="B92" s="78" t="s">
+        <v>37</v>
+      </c>
+      <c r="C92" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="64">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="E92" s="70">
+        <v>7.39</v>
+      </c>
+      <c r="F92" s="70">
+        <v>55</v>
+      </c>
+      <c r="G92" s="79">
+        <v>6050</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7">
+      <c r="B93" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="64">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="E93" s="70">
+        <v>6.35</v>
+      </c>
+      <c r="F93" s="70">
+        <v>36</v>
+      </c>
+      <c r="G93" s="79">
+        <v>5998</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7">
+      <c r="B94" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="64">
+        <v>3.2440000000000002</v>
+      </c>
+      <c r="E94" s="70">
+        <v>106.16</v>
+      </c>
+      <c r="F94" s="70">
+        <v>70</v>
+      </c>
+      <c r="G94" s="79">
+        <v>127852</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7">
+      <c r="B95" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95" s="64">
+        <v>1.88</v>
+      </c>
+      <c r="E95" s="70">
+        <v>91.88</v>
+      </c>
+      <c r="F95" s="70">
+        <v>70</v>
+      </c>
+      <c r="G95" s="79">
+        <v>133303</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" ht="20" thickBot="1">
+      <c r="B96" s="80" t="s">
+        <v>41</v>
+      </c>
+      <c r="C96" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" s="65">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="E96" s="71">
+        <v>15.48</v>
+      </c>
+      <c r="F96" s="71">
+        <v>93</v>
+      </c>
+      <c r="G96" s="81">
+        <v>9762</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7">
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B80:G80"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B32:G32"/>

</xml_diff>

<commit_message>
2 benchmarks complete, ready for heuristic3 -- run with heuristic3.sh
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sejaldua/Desktop/DIS/AI/sejelo-searchclient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004BBE42-8160-494D-A393-EAC9894C9031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5627DCDE-1702-C240-BE22-42E55EFF0D50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="600" windowWidth="20000" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
+    <workbookView xWindow="16440" yWindow="460" windowWidth="14440" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="51">
   <si>
     <t>Level</t>
   </si>
@@ -160,12 +160,39 @@
   </si>
   <si>
     <t>Table 6: Benchmarks for Sokoban Levels - Exercise 4</t>
+  </si>
+  <si>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t>A*</t>
+  </si>
+  <si>
+    <t>Greedy</t>
+  </si>
+  <si>
+    <t>SAsoko1_64.lvl</t>
+  </si>
+  <si>
+    <t>SAsoko2_64.lvl</t>
+  </si>
+  <si>
+    <t>SAsoko3_64.lvl</t>
+  </si>
+  <si>
+    <t>Table 1: Heuristic Implementation #1 using best-first search client - Exercise 5</t>
+  </si>
+  <si>
+    <t>Table 2: Heuristic Implementation #2 using best-first search client - Exercise 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -191,7 +218,7 @@
       <name val="Calibri Light (Body)"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,8 +279,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4DAE1"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -708,22 +741,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,196 +820,289 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -961,9 +1113,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE4DAE1"/>
       <color rgb="FFE4F3FF"/>
       <color rgb="FFDFDCFF"/>
-      <color rgb="FFE4DAE1"/>
       <color rgb="FFFFD0B3"/>
     </mruColors>
   </colors>
@@ -1275,17 +1427,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7093C41-8786-554E-A962-A4525C17734E}">
-  <dimension ref="B1:H97"/>
+  <dimension ref="B1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="L77" sqref="L77"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="87" workbookViewId="0">
+      <selection activeCell="G133" sqref="G133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="5.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="12.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="20.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" style="1" customWidth="1"/>
@@ -1294,1768 +1447,2431 @@
   <sheetData>
     <row r="1" spans="2:8" ht="20" thickBot="1"/>
     <row r="2" spans="2:8">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="7">
         <v>0.151</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="7">
         <v>25.28</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <v>19</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="8">
         <v>80</v>
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="10">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <v>15.02</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="10">
         <v>27</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="11">
         <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>67.546999999999997</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="7">
         <v>8192</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>18195</v>
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="10">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>12.39</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="10">
         <v>25</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="11">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>58.088999999999999</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <v>8122.34</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <v>8</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <v>30799</v>
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="10">
         <v>0.17100000000000001</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <v>36.94</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="10">
         <v>60</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="11">
         <v>305</v>
       </c>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>0.45500000000000002</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="7">
         <v>135.57</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="7">
         <v>3</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="8">
         <v>1227</v>
       </c>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="10">
         <v>24.14</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="10">
         <v>8192</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="11">
         <v>30012</v>
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>27.82</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <v>8192</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="8">
         <v>81629</v>
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="10">
         <v>24.06</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="10">
         <v>8192</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="11">
         <v>87730</v>
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="7">
         <v>34.701000000000001</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="7">
         <v>8192</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="8">
         <v>87572</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="20" thickBot="1">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>19.646999999999998</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="13">
         <v>8192</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="14">
         <v>73865</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="20" thickBot="1"/>
     <row r="17" spans="2:7">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="81"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="7">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="7">
         <v>15.68</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="7">
         <v>19</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="8">
         <v>80</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="10">
         <v>0.13</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="10">
         <v>11.4</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="10">
         <v>27</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="11">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="7">
         <v>67.188999999999993</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="7">
         <v>8192</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="8">
         <v>219020</v>
       </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="10">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="10">
         <v>9.1199999999999992</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="10">
         <v>25</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="11">
         <v>86</v>
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="7">
         <v>17.149000000000001</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="7">
         <v>3307.72</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="7">
         <v>8</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="8">
         <v>89112</v>
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="10">
         <v>0.10100000000000001</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="10">
         <v>15.34</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="10">
         <v>60</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="11">
         <v>305</v>
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="7">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="7">
         <v>60.2</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="7">
         <v>3</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="8">
         <v>1227</v>
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="10">
         <v>28.762</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="10">
         <v>8192</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="11">
         <v>204410</v>
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="7">
         <v>43.664999999999999</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="7">
         <v>8192</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="8">
         <v>221864</v>
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="10">
         <v>34.055999999999997</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="10">
         <v>8192</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="11">
         <v>219263</v>
       </c>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="7">
         <v>48.133000000000003</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="7">
         <v>8192</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="8">
         <v>225596</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="20" thickBot="1">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="13">
         <v>31.986000000000001</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="13">
         <v>8192</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="17">
+      <c r="G30" s="14">
         <v>213472</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="20" thickBot="1"/>
     <row r="32" spans="2:7">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="4"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="81"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="7">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="7">
         <v>3.72</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="7">
         <v>19</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="8">
         <v>80</v>
       </c>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="10">
         <v>3.59</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F35" s="10">
         <v>27</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="11">
         <v>75</v>
       </c>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="7">
         <v>14.467000000000001</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="7">
         <v>692.72</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36" s="7">
         <v>19</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="8">
         <v>635190</v>
       </c>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="10">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="10">
         <v>3.59</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="10">
         <v>25</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="11">
         <v>86</v>
       </c>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="7">
         <v>1.1850000000000001</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="7">
         <v>72.13</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="7">
         <v>8</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="8">
         <v>89112</v>
       </c>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="10">
         <v>3.1E-2</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="10">
         <v>3.72</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F39" s="10">
         <v>60</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="11">
         <v>305</v>
       </c>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="7">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="7">
         <v>5.12</v>
       </c>
-      <c r="F40" s="10">
+      <c r="F40" s="7">
         <v>3</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G40" s="8">
         <v>1227</v>
       </c>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="10">
         <v>35.552</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="10">
         <v>2015.72</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F41" s="10">
         <v>981528</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="11">
         <v>2953986</v>
       </c>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="7">
         <v>18.260999999999999</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="7">
         <v>2252.7199999999998</v>
       </c>
-      <c r="F42" s="10">
+      <c r="F42" s="7">
         <v>60</v>
       </c>
-      <c r="G42" s="10">
+      <c r="G42" s="7">
         <v>1961416</v>
       </c>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="13">
+      <c r="D43" s="10">
         <v>24.539000000000001</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="10">
         <v>4101.72</v>
       </c>
-      <c r="F43" s="13">
+      <c r="F43" s="10">
         <v>2517074</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="11">
         <v>4089953</v>
       </c>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="7">
         <v>179.98599999999999</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="7">
         <v>3840.72</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G44" s="11">
+      <c r="G44" s="8">
         <v>6464388</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="20" thickBot="1">
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="13">
         <v>9.218</v>
       </c>
-      <c r="E45" s="16">
+      <c r="E45" s="13">
         <v>4392.28</v>
       </c>
-      <c r="F45" s="16">
+      <c r="F45" s="13">
         <v>380992</v>
       </c>
-      <c r="G45" s="17">
+      <c r="G45" s="14">
         <v>1023377</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="20" thickBot="1"/>
     <row r="47" spans="2:7">
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="4"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="80"/>
+      <c r="F47" s="80"/>
+      <c r="G47" s="81"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="19" t="s">
+      <c r="B48" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E48" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="F48" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G48" s="22" t="s">
+      <c r="G48" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="34" t="s">
+      <c r="B49" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="35">
+      <c r="C49" s="31">
         <v>4</v>
       </c>
-      <c r="D49" s="36">
+      <c r="D49" s="32">
         <v>1.6E-2</v>
       </c>
-      <c r="E49" s="37">
+      <c r="E49" s="33">
         <v>3.59</v>
       </c>
-      <c r="F49" s="37">
+      <c r="F49" s="33">
         <v>2</v>
       </c>
-      <c r="G49" s="38">
+      <c r="G49" s="34">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="39" t="s">
+      <c r="B50" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="40">
+      <c r="C50" s="36">
         <v>8</v>
       </c>
-      <c r="D50" s="41">
+      <c r="D50" s="37">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E50" s="42">
+      <c r="E50" s="38">
         <v>3.59</v>
       </c>
-      <c r="F50" s="42">
+      <c r="F50" s="38">
         <v>6</v>
       </c>
-      <c r="G50" s="43">
+      <c r="G50" s="39">
         <v>15</v>
       </c>
     </row>
     <row r="51" spans="2:7">
-      <c r="B51" s="39" t="s">
+      <c r="B51" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="40">
+      <c r="C51" s="36">
         <v>16</v>
       </c>
-      <c r="D51" s="41">
+      <c r="D51" s="37">
         <v>2.4E-2</v>
       </c>
-      <c r="E51" s="42">
+      <c r="E51" s="38">
         <v>3.59</v>
       </c>
-      <c r="F51" s="42">
+      <c r="F51" s="38">
         <v>14</v>
       </c>
-      <c r="G51" s="43">
+      <c r="G51" s="39">
         <v>68</v>
       </c>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="39" t="s">
+      <c r="B52" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="40">
+      <c r="C52" s="36">
         <v>32</v>
       </c>
-      <c r="D52" s="41">
+      <c r="D52" s="37">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E52" s="42">
+      <c r="E52" s="38">
         <v>4</v>
       </c>
-      <c r="F52" s="42">
+      <c r="F52" s="38">
         <v>30</v>
       </c>
-      <c r="G52" s="43">
+      <c r="G52" s="39">
         <v>266</v>
       </c>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="39" t="s">
+      <c r="B53" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="40">
+      <c r="C53" s="36">
         <v>64</v>
       </c>
-      <c r="D53" s="41">
+      <c r="D53" s="37">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E53" s="42">
+      <c r="E53" s="38">
         <v>6.28</v>
       </c>
-      <c r="F53" s="42">
+      <c r="F53" s="38">
         <v>62</v>
       </c>
-      <c r="G53" s="43">
+      <c r="G53" s="39">
         <v>1034</v>
       </c>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="44" t="s">
+      <c r="B54" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="45">
+      <c r="C54" s="41">
         <v>128</v>
       </c>
-      <c r="D54" s="46">
+      <c r="D54" s="42">
         <v>0.15</v>
       </c>
-      <c r="E54" s="47">
+      <c r="E54" s="43">
         <v>10.09</v>
       </c>
-      <c r="F54" s="47">
+      <c r="F54" s="43">
         <v>126</v>
       </c>
-      <c r="G54" s="48">
+      <c r="G54" s="44">
         <v>4128</v>
       </c>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="24" t="s">
+      <c r="B55" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="25">
+      <c r="C55" s="21">
         <v>4</v>
       </c>
-      <c r="D55" s="26">
+      <c r="D55" s="22">
         <v>1.9E-2</v>
       </c>
-      <c r="E55" s="27">
+      <c r="E55" s="23">
         <v>3.59</v>
       </c>
-      <c r="F55" s="27">
+      <c r="F55" s="23">
         <v>2</v>
       </c>
-      <c r="G55" s="28">
+      <c r="G55" s="24">
         <v>44</v>
       </c>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="29" t="s">
+      <c r="B56" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="30">
+      <c r="C56" s="26">
         <v>8</v>
       </c>
-      <c r="D56" s="31">
+      <c r="D56" s="27">
         <v>4.7E-2</v>
       </c>
-      <c r="E56" s="32">
+      <c r="E56" s="28">
         <v>5.4</v>
       </c>
-      <c r="F56" s="32">
+      <c r="F56" s="28">
         <v>6</v>
       </c>
-      <c r="G56" s="33">
+      <c r="G56" s="29">
         <v>660</v>
       </c>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C57" s="30">
+      <c r="C57" s="26">
         <v>16</v>
       </c>
-      <c r="D57" s="31">
+      <c r="D57" s="27">
         <v>0.32900000000000001</v>
       </c>
-      <c r="E57" s="32">
+      <c r="E57" s="28">
         <v>21.27</v>
       </c>
-      <c r="F57" s="32">
+      <c r="F57" s="28">
         <v>14</v>
       </c>
-      <c r="G57" s="33">
+      <c r="G57" s="29">
         <v>8580</v>
       </c>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="30">
+      <c r="C58" s="26">
         <v>32</v>
       </c>
-      <c r="D58" s="31">
+      <c r="D58" s="27">
         <v>3.6859999999999999</v>
       </c>
-      <c r="E58" s="32">
+      <c r="E58" s="28">
         <v>515.72</v>
       </c>
-      <c r="F58" s="32">
+      <c r="F58" s="28">
         <v>30</v>
       </c>
-      <c r="G58" s="33">
+      <c r="G58" s="29">
         <v>118093</v>
       </c>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="49" t="s">
+      <c r="B59" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="50">
+      <c r="C59" s="46">
         <v>64</v>
       </c>
-      <c r="D59" s="51">
+      <c r="D59" s="47">
         <v>98.825000000000003</v>
       </c>
-      <c r="E59" s="52">
+      <c r="E59" s="48">
         <v>8192</v>
       </c>
-      <c r="F59" s="52" t="s">
+      <c r="F59" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G59" s="53">
+      <c r="G59" s="49">
         <v>808491</v>
       </c>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="59" t="s">
+      <c r="B60" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="60">
+      <c r="C60" s="56">
         <v>128</v>
       </c>
-      <c r="D60" s="61">
+      <c r="D60" s="57">
         <v>65.835999999999999</v>
       </c>
-      <c r="E60" s="62">
+      <c r="E60" s="58">
         <v>8192</v>
       </c>
-      <c r="F60" s="62" t="s">
+      <c r="F60" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="G60" s="63">
+      <c r="G60" s="59">
         <v>221993</v>
       </c>
     </row>
     <row r="61" spans="2:7">
-      <c r="B61" s="39" t="s">
+      <c r="B61" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C61" s="40">
+      <c r="C61" s="36">
         <v>4</v>
       </c>
-      <c r="D61" s="41">
+      <c r="D61" s="37">
         <v>0.42899999999999999</v>
       </c>
-      <c r="E61" s="42">
+      <c r="E61" s="38">
         <v>11.63</v>
       </c>
-      <c r="F61" s="42">
+      <c r="F61" s="38">
         <v>8</v>
       </c>
-      <c r="G61" s="43">
+      <c r="G61" s="39">
         <v>17016</v>
       </c>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="39" t="s">
+      <c r="B62" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C62" s="40">
+      <c r="C62" s="36">
         <v>5</v>
       </c>
-      <c r="D62" s="41">
+      <c r="D62" s="37">
         <v>60.161000000000001</v>
       </c>
-      <c r="E62" s="42">
+      <c r="E62" s="38">
         <v>820.72</v>
       </c>
-      <c r="F62" s="42">
+      <c r="F62" s="38">
         <v>15</v>
       </c>
-      <c r="G62" s="43">
+      <c r="G62" s="39">
         <v>874805</v>
       </c>
     </row>
     <row r="63" spans="2:7">
-      <c r="B63" s="49" t="s">
+      <c r="B63" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C63" s="50">
+      <c r="C63" s="46">
         <v>6</v>
       </c>
-      <c r="D63" s="51">
+      <c r="D63" s="47">
         <v>178.28</v>
       </c>
-      <c r="E63" s="52">
+      <c r="E63" s="48">
         <v>1900.72</v>
       </c>
-      <c r="F63" s="52" t="s">
+      <c r="F63" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G63" s="53">
+      <c r="G63" s="49">
         <v>3287110</v>
       </c>
     </row>
     <row r="64" spans="2:7">
-      <c r="B64" s="49" t="s">
+      <c r="B64" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C64" s="50">
+      <c r="C64" s="46">
         <v>7</v>
       </c>
-      <c r="D64" s="51">
+      <c r="D64" s="47">
         <v>178.01</v>
       </c>
-      <c r="E64" s="52">
+      <c r="E64" s="48">
         <v>2834.72</v>
       </c>
-      <c r="F64" s="52" t="s">
+      <c r="F64" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G64" s="52">
+      <c r="G64" s="48">
         <v>4032039</v>
       </c>
     </row>
     <row r="65" spans="2:7">
-      <c r="B65" s="49" t="s">
+      <c r="B65" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C65" s="50">
+      <c r="C65" s="46">
         <v>8</v>
       </c>
-      <c r="D65" s="51">
+      <c r="D65" s="47">
         <v>179.13</v>
       </c>
-      <c r="E65" s="52">
+      <c r="E65" s="48">
         <v>3482.72</v>
       </c>
-      <c r="F65" s="52" t="s">
+      <c r="F65" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="53">
+      <c r="G65" s="49">
         <v>4734372</v>
       </c>
     </row>
     <row r="66" spans="2:7">
-      <c r="B66" s="49" t="s">
+      <c r="B66" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="50">
+      <c r="C66" s="46">
         <v>16</v>
       </c>
-      <c r="D66" s="51">
+      <c r="D66" s="47">
         <v>178.7</v>
       </c>
-      <c r="E66" s="52">
+      <c r="E66" s="48">
         <v>6819.72</v>
       </c>
-      <c r="F66" s="52" t="s">
+      <c r="F66" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G66" s="53">
+      <c r="G66" s="49">
         <v>5173127</v>
       </c>
     </row>
     <row r="67" spans="2:7">
-      <c r="B67" s="49" t="s">
+      <c r="B67" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C67" s="50">
+      <c r="C67" s="46">
         <v>32</v>
       </c>
-      <c r="D67" s="51">
+      <c r="D67" s="47">
         <v>93.528000000000006</v>
       </c>
-      <c r="E67" s="52">
+      <c r="E67" s="48">
         <v>8192</v>
       </c>
-      <c r="F67" s="52" t="s">
+      <c r="F67" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G67" s="53">
+      <c r="G67" s="49">
         <v>2506572</v>
       </c>
     </row>
     <row r="68" spans="2:7">
-      <c r="B68" s="49" t="s">
+      <c r="B68" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C68" s="50">
+      <c r="C68" s="46">
         <v>64</v>
       </c>
-      <c r="D68" s="51">
+      <c r="D68" s="47">
         <v>57.46</v>
       </c>
-      <c r="E68" s="52">
+      <c r="E68" s="48">
         <v>8192</v>
       </c>
-      <c r="F68" s="52" t="s">
+      <c r="F68" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G68" s="53">
+      <c r="G68" s="49">
         <v>810381</v>
       </c>
     </row>
     <row r="69" spans="2:7" ht="20" thickBot="1">
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C69" s="55">
+      <c r="C69" s="51">
         <v>128</v>
       </c>
-      <c r="D69" s="56">
+      <c r="D69" s="52">
         <v>35.396999999999998</v>
       </c>
-      <c r="E69" s="57">
+      <c r="E69" s="53">
         <v>8192</v>
       </c>
-      <c r="F69" s="57" t="s">
+      <c r="F69" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G69" s="58">
+      <c r="G69" s="54">
         <v>224619</v>
       </c>
     </row>
     <row r="70" spans="2:7" ht="20" thickBot="1"/>
     <row r="71" spans="2:7">
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="4"/>
+      <c r="C71" s="80"/>
+      <c r="D71" s="80"/>
+      <c r="E71" s="80"/>
+      <c r="F71" s="80"/>
+      <c r="G71" s="81"/>
     </row>
     <row r="72" spans="2:7">
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E72" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="F72" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G72" s="8" t="s">
+      <c r="G72" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="73" spans="2:7">
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="10">
+      <c r="D73" s="7">
         <v>0.21299999999999999</v>
       </c>
-      <c r="E73" s="10">
+      <c r="E73" s="7">
         <v>20.11</v>
       </c>
-      <c r="F73" s="10">
+      <c r="F73" s="7">
         <v>676</v>
       </c>
-      <c r="G73" s="11">
+      <c r="G73" s="8">
         <v>1753</v>
       </c>
     </row>
     <row r="74" spans="2:7">
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D74" s="13">
+      <c r="D74" s="10">
         <v>0.14399999999999999</v>
       </c>
-      <c r="E74" s="13">
+      <c r="E74" s="10">
         <v>17.97</v>
       </c>
-      <c r="F74" s="13">
+      <c r="F74" s="10">
         <v>676</v>
       </c>
-      <c r="G74" s="14">
+      <c r="G74" s="11">
         <v>1082</v>
       </c>
     </row>
     <row r="75" spans="2:7">
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C75" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="10">
+      <c r="D75" s="7">
         <v>0.17</v>
       </c>
-      <c r="E75" s="10">
+      <c r="E75" s="7">
         <v>10.66</v>
       </c>
-      <c r="F75" s="10">
+      <c r="F75" s="7">
         <v>1110</v>
       </c>
-      <c r="G75" s="11">
+      <c r="G75" s="8">
         <v>1150</v>
       </c>
     </row>
     <row r="76" spans="2:7">
-      <c r="B76" s="12" t="s">
+      <c r="B76" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D76" s="13">
+      <c r="D76" s="10">
         <v>0.122</v>
       </c>
-      <c r="E76" s="13">
+      <c r="E76" s="10">
         <v>10.78</v>
       </c>
-      <c r="F76" s="13">
+      <c r="F76" s="10">
         <v>1110</v>
       </c>
-      <c r="G76" s="14">
+      <c r="G76" s="11">
         <v>1150</v>
       </c>
     </row>
     <row r="77" spans="2:7">
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C77" s="10" t="s">
+      <c r="C77" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D77" s="10">
+      <c r="D77" s="7">
         <v>0.13</v>
       </c>
-      <c r="E77" s="10">
+      <c r="E77" s="7">
         <v>9.1199999999999992</v>
       </c>
-      <c r="F77" s="10">
+      <c r="F77" s="7">
         <v>112</v>
       </c>
-      <c r="G77" s="11">
+      <c r="G77" s="8">
         <v>535</v>
       </c>
     </row>
     <row r="78" spans="2:7" ht="20" thickBot="1">
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C78" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D78" s="16">
+      <c r="D78" s="13">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="E78" s="16">
+      <c r="E78" s="13">
         <v>7.4</v>
       </c>
-      <c r="F78" s="16">
+      <c r="F78" s="13">
         <v>154</v>
       </c>
-      <c r="G78" s="17">
+      <c r="G78" s="14">
         <v>396</v>
       </c>
     </row>
     <row r="79" spans="2:7" ht="20" thickBot="1">
-      <c r="B79" s="23"/>
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
-      <c r="E79" s="23"/>
-      <c r="F79" s="23"/>
-      <c r="G79" s="23"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
     </row>
     <row r="80" spans="2:7">
-      <c r="B80" s="72" t="s">
+      <c r="B80" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="C80" s="18"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="73"/>
+      <c r="C80" s="77"/>
+      <c r="D80" s="77"/>
+      <c r="E80" s="77"/>
+      <c r="F80" s="77"/>
+      <c r="G80" s="78"/>
     </row>
     <row r="81" spans="2:7">
-      <c r="B81" s="6" t="s">
+      <c r="B81" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="C81" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E81" s="7" t="s">
+      <c r="E81" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F81" s="7" t="s">
+      <c r="F81" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G81" s="8" t="s">
+      <c r="G81" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="82" spans="2:7">
-      <c r="B82" s="74" t="s">
+      <c r="B82" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="C82" s="67" t="s">
+      <c r="C82" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D82" s="67">
+      <c r="D82" s="63">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="E82" s="68">
+      <c r="E82" s="64">
         <v>5.12</v>
       </c>
-      <c r="F82" s="68">
+      <c r="F82" s="64">
         <v>34</v>
       </c>
-      <c r="G82" s="75">
+      <c r="G82" s="69">
         <v>749</v>
       </c>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" s="74" t="s">
+      <c r="B83" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="C83" s="67" t="s">
+      <c r="C83" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D83" s="67">
+      <c r="D83" s="63">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="E83" s="68">
+      <c r="E83" s="64">
         <v>7.68</v>
       </c>
-      <c r="F83" s="68">
+      <c r="F83" s="64">
         <v>23</v>
       </c>
-      <c r="G83" s="75">
+      <c r="G83" s="69">
         <v>1983</v>
       </c>
     </row>
     <row r="84" spans="2:7">
-      <c r="B84" s="74" t="s">
+      <c r="B84" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="C84" s="67" t="s">
+      <c r="C84" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D84" s="67">
+      <c r="D84" s="63">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="E84" s="68">
+      <c r="E84" s="64">
         <v>10.28</v>
       </c>
-      <c r="F84" s="68">
+      <c r="F84" s="64">
         <v>31</v>
       </c>
-      <c r="G84" s="75">
+      <c r="G84" s="69">
         <v>2960</v>
       </c>
     </row>
     <row r="85" spans="2:7">
-      <c r="B85" s="74" t="s">
+      <c r="B85" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="C85" s="67" t="s">
+      <c r="C85" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D85" s="67">
+      <c r="D85" s="63">
         <v>0.253</v>
       </c>
-      <c r="E85" s="68">
+      <c r="E85" s="64">
         <v>21.74</v>
       </c>
-      <c r="F85" s="68">
+      <c r="F85" s="64">
         <v>25</v>
       </c>
-      <c r="G85" s="75">
+      <c r="G85" s="69">
         <v>12520</v>
       </c>
     </row>
     <row r="86" spans="2:7">
-      <c r="B86" s="74" t="s">
+      <c r="B86" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="C86" s="67" t="s">
+      <c r="C86" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D86" s="67">
+      <c r="D86" s="63">
         <v>0.46100000000000002</v>
       </c>
-      <c r="E86" s="68">
+      <c r="E86" s="64">
         <v>29.66</v>
       </c>
-      <c r="F86" s="68">
+      <c r="F86" s="64">
         <v>37</v>
       </c>
-      <c r="G86" s="75">
+      <c r="G86" s="69">
         <v>22718</v>
       </c>
     </row>
     <row r="87" spans="2:7">
-      <c r="B87" s="76" t="s">
+      <c r="B87" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="C87" s="66" t="s">
+      <c r="C87" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="D87" s="66">
+      <c r="D87" s="62">
         <v>0.16600000000000001</v>
       </c>
-      <c r="E87" s="69">
+      <c r="E87" s="65">
         <v>10.35</v>
       </c>
-      <c r="F87" s="69">
+      <c r="F87" s="65">
         <v>53</v>
       </c>
-      <c r="G87" s="77">
+      <c r="G87" s="71">
         <v>8061</v>
       </c>
     </row>
     <row r="88" spans="2:7">
-      <c r="B88" s="76" t="s">
+      <c r="B88" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="C88" s="66" t="s">
+      <c r="C88" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="D88" s="66">
+      <c r="D88" s="62">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E88" s="69">
+      <c r="E88" s="65">
         <v>24.18</v>
       </c>
-      <c r="F88" s="69">
+      <c r="F88" s="65">
         <v>59</v>
       </c>
-      <c r="G88" s="77">
+      <c r="G88" s="71">
         <v>18041</v>
       </c>
     </row>
     <row r="89" spans="2:7">
-      <c r="B89" s="76" t="s">
+      <c r="B89" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="C89" s="66" t="s">
+      <c r="C89" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="D89" s="66">
+      <c r="D89" s="62">
         <v>0.73099999999999998</v>
       </c>
-      <c r="E89" s="69">
+      <c r="E89" s="65">
         <v>29.24</v>
       </c>
-      <c r="F89" s="69">
+      <c r="F89" s="65">
         <v>53</v>
       </c>
-      <c r="G89" s="77">
+      <c r="G89" s="71">
         <v>40349</v>
       </c>
     </row>
     <row r="90" spans="2:7">
-      <c r="B90" s="76" t="s">
+      <c r="B90" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C90" s="66" t="s">
+      <c r="C90" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="D90" s="66">
+      <c r="D90" s="62">
         <v>0.184</v>
       </c>
-      <c r="E90" s="69">
+      <c r="E90" s="65">
         <v>7.21</v>
       </c>
-      <c r="F90" s="69">
+      <c r="F90" s="65">
         <v>75</v>
       </c>
-      <c r="G90" s="77">
+      <c r="G90" s="71">
         <v>6358</v>
       </c>
     </row>
     <row r="91" spans="2:7">
-      <c r="B91" s="76" t="s">
+      <c r="B91" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="C91" s="66" t="s">
+      <c r="C91" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="D91" s="66">
+      <c r="D91" s="62">
         <v>0.17399999999999999</v>
       </c>
-      <c r="E91" s="69">
+      <c r="E91" s="65">
         <v>12.54</v>
       </c>
-      <c r="F91" s="69">
+      <c r="F91" s="65">
         <v>60</v>
       </c>
-      <c r="G91" s="77">
+      <c r="G91" s="71">
         <v>7817</v>
       </c>
     </row>
     <row r="92" spans="2:7">
-      <c r="B92" s="78" t="s">
+      <c r="B92" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="C92" s="64" t="s">
+      <c r="C92" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D92" s="64">
+      <c r="D92" s="60">
         <v>0.34399999999999997</v>
       </c>
-      <c r="E92" s="70">
+      <c r="E92" s="66">
         <v>7.39</v>
       </c>
-      <c r="F92" s="70">
+      <c r="F92" s="66">
         <v>55</v>
       </c>
-      <c r="G92" s="79">
+      <c r="G92" s="73">
         <v>6050</v>
       </c>
     </row>
     <row r="93" spans="2:7">
-      <c r="B93" s="78" t="s">
+      <c r="B93" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="C93" s="64" t="s">
+      <c r="C93" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D93" s="64">
+      <c r="D93" s="60">
         <v>0.14699999999999999</v>
       </c>
-      <c r="E93" s="70">
+      <c r="E93" s="66">
         <v>6.35</v>
       </c>
-      <c r="F93" s="70">
+      <c r="F93" s="66">
         <v>36</v>
       </c>
-      <c r="G93" s="79">
+      <c r="G93" s="73">
         <v>5998</v>
       </c>
     </row>
     <row r="94" spans="2:7">
-      <c r="B94" s="78" t="s">
+      <c r="B94" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="C94" s="64" t="s">
+      <c r="C94" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D94" s="64">
+      <c r="D94" s="60">
         <v>3.2440000000000002</v>
       </c>
-      <c r="E94" s="70">
+      <c r="E94" s="66">
         <v>106.16</v>
       </c>
-      <c r="F94" s="70">
+      <c r="F94" s="66">
         <v>70</v>
       </c>
-      <c r="G94" s="79">
+      <c r="G94" s="73">
         <v>127852</v>
       </c>
     </row>
     <row r="95" spans="2:7">
-      <c r="B95" s="78" t="s">
+      <c r="B95" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="C95" s="64" t="s">
+      <c r="C95" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D95" s="64">
+      <c r="D95" s="60">
         <v>1.88</v>
       </c>
-      <c r="E95" s="70">
+      <c r="E95" s="66">
         <v>91.88</v>
       </c>
-      <c r="F95" s="70">
+      <c r="F95" s="66">
         <v>70</v>
       </c>
-      <c r="G95" s="79">
+      <c r="G95" s="73">
         <v>133303</v>
       </c>
     </row>
     <row r="96" spans="2:7" ht="20" thickBot="1">
-      <c r="B96" s="80" t="s">
+      <c r="B96" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="C96" s="65" t="s">
+      <c r="C96" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="D96" s="65">
+      <c r="D96" s="61">
         <v>0.24099999999999999</v>
       </c>
-      <c r="E96" s="71">
+      <c r="E96" s="67">
         <v>15.48</v>
       </c>
-      <c r="F96" s="71">
+      <c r="F96" s="67">
         <v>93</v>
       </c>
-      <c r="G96" s="81">
+      <c r="G96" s="75">
         <v>9762</v>
       </c>
     </row>
-    <row r="97" spans="2:7">
-      <c r="B97" s="23"/>
-      <c r="C97" s="23"/>
-      <c r="D97" s="23"/>
-      <c r="E97" s="23"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="23"/>
+    <row r="97" spans="2:7" ht="20" thickBot="1">
+      <c r="B97" s="19"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="19"/>
+      <c r="G97" s="19"/>
+    </row>
+    <row r="98" spans="2:7">
+      <c r="B98" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="C98" s="80"/>
+      <c r="D98" s="80"/>
+      <c r="E98" s="80"/>
+      <c r="F98" s="80"/>
+      <c r="G98" s="81"/>
+    </row>
+    <row r="99" spans="2:7">
+      <c r="B99" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D99" s="85" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="85" t="s">
+        <v>2</v>
+      </c>
+      <c r="G99" s="95" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7">
+      <c r="B100" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D100" s="86">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="E100" s="89">
+        <v>4</v>
+      </c>
+      <c r="F100" s="92">
+        <v>19</v>
+      </c>
+      <c r="G100" s="97">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7">
+      <c r="B101" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C101" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D101" s="87">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="E101" s="90">
+        <v>3.62</v>
+      </c>
+      <c r="F101" s="93">
+        <v>21</v>
+      </c>
+      <c r="G101" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7">
+      <c r="B102" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D102" s="88">
+        <v>41.015000000000001</v>
+      </c>
+      <c r="E102" s="91">
+        <v>940.72</v>
+      </c>
+      <c r="F102" s="94">
+        <v>19</v>
+      </c>
+      <c r="G102" s="8">
+        <v>359928</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7">
+      <c r="B103" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D103" s="87">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="E103" s="90">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="F103" s="93">
+        <v>53</v>
+      </c>
+      <c r="G103" s="11">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7">
+      <c r="B104" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D104" s="88">
+        <v>2.82</v>
+      </c>
+      <c r="E104" s="91">
+        <v>75.930000000000007</v>
+      </c>
+      <c r="F104" s="94">
+        <v>8</v>
+      </c>
+      <c r="G104" s="8">
+        <v>35432</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7">
+      <c r="B105" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D105" s="87">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E105" s="90">
+        <v>3.62</v>
+      </c>
+      <c r="F105" s="93">
+        <v>10</v>
+      </c>
+      <c r="G105" s="11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7">
+      <c r="B106" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D106" s="88">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E106" s="91">
+        <v>3.34</v>
+      </c>
+      <c r="F106" s="94">
+        <v>3</v>
+      </c>
+      <c r="G106" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7">
+      <c r="B107" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D107" s="87">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E107" s="90">
+        <v>3.34</v>
+      </c>
+      <c r="F107" s="93">
+        <v>3</v>
+      </c>
+      <c r="G107" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7">
+      <c r="B108" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D108" s="88">
+        <v>2.5550000000000002</v>
+      </c>
+      <c r="E108" s="91">
+        <v>121.3</v>
+      </c>
+      <c r="F108" s="94">
+        <v>60</v>
+      </c>
+      <c r="G108" s="8">
+        <v>9209</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7">
+      <c r="B109" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D109" s="87">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="E109" s="90">
+        <v>15.68</v>
+      </c>
+      <c r="F109" s="93">
+        <v>99</v>
+      </c>
+      <c r="G109" s="11">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7">
+      <c r="B110" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C110" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D110" s="88">
+        <v>180</v>
+      </c>
+      <c r="E110" s="91">
+        <v>1317.82</v>
+      </c>
+      <c r="F110" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G110" s="8">
+        <v>1888924</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7">
+      <c r="B111" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D111" s="87">
+        <v>8.0129999999999999</v>
+      </c>
+      <c r="E111" s="90">
+        <v>554.48</v>
+      </c>
+      <c r="F111" s="93">
+        <v>140</v>
+      </c>
+      <c r="G111" s="11">
+        <v>166347</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7">
+      <c r="B112" s="98" t="s">
+        <v>46</v>
+      </c>
+      <c r="C112" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="D112" s="100">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E112" s="101">
+        <v>4.84</v>
+      </c>
+      <c r="F112" s="102">
+        <v>62</v>
+      </c>
+      <c r="G112" s="103">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7">
+      <c r="B113" s="98" t="s">
+        <v>47</v>
+      </c>
+      <c r="C113" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="D113" s="100">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E113" s="101">
+        <v>10.84</v>
+      </c>
+      <c r="F113" s="102">
+        <v>62</v>
+      </c>
+      <c r="G113" s="103">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" ht="20" thickBot="1">
+      <c r="B114" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="C114" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="D114" s="106">
+        <v>172.18299999999999</v>
+      </c>
+      <c r="E114" s="107">
+        <v>8192</v>
+      </c>
+      <c r="F114" s="108" t="s">
+        <v>14</v>
+      </c>
+      <c r="G114" s="109">
+        <v>813831</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" ht="20" thickBot="1"/>
+    <row r="116" spans="2:7">
+      <c r="B116" s="79" t="s">
+        <v>50</v>
+      </c>
+      <c r="C116" s="80"/>
+      <c r="D116" s="80"/>
+      <c r="E116" s="80"/>
+      <c r="F116" s="80"/>
+      <c r="G116" s="81"/>
+    </row>
+    <row r="117" spans="2:7">
+      <c r="B117" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D117" s="85" t="s">
+        <v>12</v>
+      </c>
+      <c r="E117" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="F117" s="85" t="s">
+        <v>2</v>
+      </c>
+      <c r="G117" s="95" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7">
+      <c r="B118" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D118" s="86">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E118" s="89">
+        <v>3.65</v>
+      </c>
+      <c r="F118" s="92">
+        <v>19</v>
+      </c>
+      <c r="G118" s="97">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7">
+      <c r="B119" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C119" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D119" s="87">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="E119" s="90">
+        <v>3.65</v>
+      </c>
+      <c r="F119" s="93">
+        <v>21</v>
+      </c>
+      <c r="G119" s="11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7">
+      <c r="B120" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D120" s="88">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="E120" s="91">
+        <v>8.56</v>
+      </c>
+      <c r="F120" s="94">
+        <v>19</v>
+      </c>
+      <c r="G120" s="8">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7">
+      <c r="B121" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D121" s="87">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="E121" s="90">
+        <v>3.65</v>
+      </c>
+      <c r="F121" s="93">
+        <v>21</v>
+      </c>
+      <c r="G121" s="11">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7">
+      <c r="B122" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D122" s="88">
+        <v>1.35</v>
+      </c>
+      <c r="E122" s="91">
+        <v>37.270000000000003</v>
+      </c>
+      <c r="F122" s="94">
+        <v>8</v>
+      </c>
+      <c r="G122" s="8">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7">
+      <c r="B123" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D123" s="87">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="E123" s="90">
+        <v>3.72</v>
+      </c>
+      <c r="F123" s="93">
+        <v>8</v>
+      </c>
+      <c r="G123" s="11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7">
+      <c r="B124" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D124" s="88">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E124" s="91">
+        <v>3.37</v>
+      </c>
+      <c r="F124" s="94">
+        <v>3</v>
+      </c>
+      <c r="G124" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7">
+      <c r="B125" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D125" s="87">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="E125" s="90">
+        <v>3.37</v>
+      </c>
+      <c r="F125" s="93">
+        <v>3</v>
+      </c>
+      <c r="G125" s="11">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7">
+      <c r="B126" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C126" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D126" s="88">
+        <v>5.1269999999999998</v>
+      </c>
+      <c r="E126" s="91">
+        <v>162.5</v>
+      </c>
+      <c r="F126" s="94">
+        <v>62</v>
+      </c>
+      <c r="G126" s="8">
+        <v>49106</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7">
+      <c r="B127" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C127" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D127" s="87">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="E127" s="90">
+        <v>15.68</v>
+      </c>
+      <c r="F127" s="93">
+        <v>99</v>
+      </c>
+      <c r="G127" s="11">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7">
+      <c r="B128" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C128" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D128" s="88">
+        <v>180</v>
+      </c>
+      <c r="E128" s="91">
+        <v>1317.82</v>
+      </c>
+      <c r="F128" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G128" s="8">
+        <v>1888924</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7">
+      <c r="B129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C129" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D129" s="87">
+        <v>3.1920000000000002</v>
+      </c>
+      <c r="E129" s="90">
+        <v>62.35</v>
+      </c>
+      <c r="F129" s="93">
+        <v>240</v>
+      </c>
+      <c r="G129" s="11">
+        <v>19353</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7">
+      <c r="B130" s="98" t="s">
+        <v>46</v>
+      </c>
+      <c r="C130" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="D130" s="100">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="E130" s="101">
+        <v>4</v>
+      </c>
+      <c r="F130" s="102">
+        <v>62</v>
+      </c>
+      <c r="G130" s="103">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7">
+      <c r="B131" s="98" t="s">
+        <v>47</v>
+      </c>
+      <c r="C131" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="D131" s="100">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="E131" s="101">
+        <v>9.4</v>
+      </c>
+      <c r="F131" s="102">
+        <v>62</v>
+      </c>
+      <c r="G131" s="103">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" ht="20" thickBot="1">
+      <c r="B132" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="C132" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="D132" s="106">
+        <v>180</v>
+      </c>
+      <c r="E132" s="107">
+        <v>668.72</v>
+      </c>
+      <c r="F132" s="108" t="s">
+        <v>14</v>
+      </c>
+      <c r="G132" s="109">
+        <v>59024</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="B98:G98"/>
+    <mergeCell ref="B116:G116"/>
     <mergeCell ref="B80:G80"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B17:G17"/>

</xml_diff>

<commit_message>
about to make table for heuristic3 and heuristic4
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sejaldua/Desktop/DIS/AI/sejelo-searchclient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5627DCDE-1702-C240-BE22-42E55EFF0D50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{65B8791E-AE28-0745-874A-E9B3ABD8973F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16440" yWindow="460" windowWidth="14440" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
+    <workbookView xWindow="13160" yWindow="460" windowWidth="14440" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1003,6 +1003,99 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1010,99 +1103,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1447,14 +1447,14 @@
   <sheetData>
     <row r="1" spans="2:8" ht="20" thickBot="1"/>
     <row r="2" spans="2:8">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="81"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="106"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8">
@@ -1719,14 +1719,14 @@
     </row>
     <row r="16" spans="2:8" ht="20" thickBot="1"/>
     <row r="17" spans="2:7">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="106"/>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="3" t="s">
@@ -1990,14 +1990,14 @@
     </row>
     <row r="31" spans="2:7" ht="20" thickBot="1"/>
     <row r="32" spans="2:7">
-      <c r="B32" s="79" t="s">
+      <c r="B32" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="81"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="105"/>
+      <c r="E32" s="105"/>
+      <c r="F32" s="105"/>
+      <c r="G32" s="106"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="3" t="s">
@@ -2261,14 +2261,14 @@
     </row>
     <row r="46" spans="2:7" ht="20" thickBot="1"/>
     <row r="47" spans="2:7">
-      <c r="B47" s="79" t="s">
+      <c r="B47" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="77"/>
-      <c r="D47" s="80"/>
-      <c r="E47" s="80"/>
-      <c r="F47" s="80"/>
-      <c r="G47" s="81"/>
+      <c r="C47" s="108"/>
+      <c r="D47" s="105"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="105"/>
+      <c r="G47" s="106"/>
     </row>
     <row r="48" spans="2:7">
       <c r="B48" s="15" t="s">
@@ -2712,14 +2712,14 @@
     </row>
     <row r="70" spans="2:7" ht="20" thickBot="1"/>
     <row r="71" spans="2:7">
-      <c r="B71" s="79" t="s">
+      <c r="B71" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="C71" s="80"/>
-      <c r="D71" s="80"/>
-      <c r="E71" s="80"/>
-      <c r="F71" s="80"/>
-      <c r="G71" s="81"/>
+      <c r="C71" s="105"/>
+      <c r="D71" s="105"/>
+      <c r="E71" s="105"/>
+      <c r="F71" s="105"/>
+      <c r="G71" s="106"/>
     </row>
     <row r="72" spans="2:7">
       <c r="B72" s="3" t="s">
@@ -2870,14 +2870,14 @@
       <c r="G79" s="19"/>
     </row>
     <row r="80" spans="2:7">
-      <c r="B80" s="76" t="s">
+      <c r="B80" s="107" t="s">
         <v>42</v>
       </c>
-      <c r="C80" s="77"/>
-      <c r="D80" s="77"/>
-      <c r="E80" s="77"/>
-      <c r="F80" s="77"/>
-      <c r="G80" s="78"/>
+      <c r="C80" s="108"/>
+      <c r="D80" s="108"/>
+      <c r="E80" s="108"/>
+      <c r="F80" s="108"/>
+      <c r="G80" s="109"/>
     </row>
     <row r="81" spans="2:7">
       <c r="B81" s="3" t="s">
@@ -3208,52 +3208,52 @@
       <c r="G97" s="19"/>
     </row>
     <row r="98" spans="2:7">
-      <c r="B98" s="79" t="s">
+      <c r="B98" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="C98" s="80"/>
-      <c r="D98" s="80"/>
-      <c r="E98" s="80"/>
-      <c r="F98" s="80"/>
-      <c r="G98" s="81"/>
+      <c r="C98" s="105"/>
+      <c r="D98" s="105"/>
+      <c r="E98" s="105"/>
+      <c r="F98" s="105"/>
+      <c r="G98" s="106"/>
     </row>
     <row r="99" spans="2:7">
-      <c r="B99" s="82" t="s">
+      <c r="B99" s="76" t="s">
         <v>0</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D99" s="85" t="s">
+      <c r="D99" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="E99" s="85" t="s">
+      <c r="E99" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="F99" s="85" t="s">
+      <c r="F99" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="G99" s="95" t="s">
+      <c r="G99" s="89" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="100" spans="2:7">
-      <c r="B100" s="96" t="s">
+      <c r="B100" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="C100" s="83" t="s">
+      <c r="C100" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D100" s="86">
+      <c r="D100" s="80">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="E100" s="89">
+      <c r="E100" s="83">
         <v>4</v>
       </c>
-      <c r="F100" s="92">
+      <c r="F100" s="86">
         <v>19</v>
       </c>
-      <c r="G100" s="97">
+      <c r="G100" s="91">
         <v>78</v>
       </c>
     </row>
@@ -3261,16 +3261,16 @@
       <c r="B101" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C101" s="84" t="s">
+      <c r="C101" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D101" s="87">
+      <c r="D101" s="81">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="E101" s="90">
+      <c r="E101" s="84">
         <v>3.62</v>
       </c>
-      <c r="F101" s="93">
+      <c r="F101" s="87">
         <v>21</v>
       </c>
       <c r="G101" s="11">
@@ -3281,16 +3281,16 @@
       <c r="B102" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C102" s="83" t="s">
+      <c r="C102" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D102" s="88">
+      <c r="D102" s="82">
         <v>41.015000000000001</v>
       </c>
-      <c r="E102" s="91">
+      <c r="E102" s="85">
         <v>940.72</v>
       </c>
-      <c r="F102" s="94">
+      <c r="F102" s="88">
         <v>19</v>
       </c>
       <c r="G102" s="8">
@@ -3301,16 +3301,16 @@
       <c r="B103" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C103" s="84" t="s">
+      <c r="C103" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D103" s="87">
+      <c r="D103" s="81">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="E103" s="90">
+      <c r="E103" s="84">
         <v>4.5599999999999996</v>
       </c>
-      <c r="F103" s="93">
+      <c r="F103" s="87">
         <v>53</v>
       </c>
       <c r="G103" s="11">
@@ -3321,16 +3321,16 @@
       <c r="B104" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C104" s="83" t="s">
+      <c r="C104" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D104" s="88">
+      <c r="D104" s="82">
         <v>2.82</v>
       </c>
-      <c r="E104" s="91">
+      <c r="E104" s="85">
         <v>75.930000000000007</v>
       </c>
-      <c r="F104" s="94">
+      <c r="F104" s="88">
         <v>8</v>
       </c>
       <c r="G104" s="8">
@@ -3341,16 +3341,16 @@
       <c r="B105" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C105" s="84" t="s">
+      <c r="C105" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D105" s="87">
+      <c r="D105" s="81">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="E105" s="90">
+      <c r="E105" s="84">
         <v>3.62</v>
       </c>
-      <c r="F105" s="93">
+      <c r="F105" s="87">
         <v>10</v>
       </c>
       <c r="G105" s="11">
@@ -3361,16 +3361,16 @@
       <c r="B106" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C106" s="83" t="s">
+      <c r="C106" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D106" s="88">
+      <c r="D106" s="82">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="E106" s="91">
+      <c r="E106" s="85">
         <v>3.34</v>
       </c>
-      <c r="F106" s="94">
+      <c r="F106" s="88">
         <v>3</v>
       </c>
       <c r="G106" s="8">
@@ -3381,16 +3381,16 @@
       <c r="B107" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C107" s="84" t="s">
+      <c r="C107" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D107" s="87">
+      <c r="D107" s="81">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="E107" s="90">
+      <c r="E107" s="84">
         <v>3.34</v>
       </c>
-      <c r="F107" s="93">
+      <c r="F107" s="87">
         <v>3</v>
       </c>
       <c r="G107" s="11">
@@ -3401,16 +3401,16 @@
       <c r="B108" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C108" s="83" t="s">
+      <c r="C108" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D108" s="88">
+      <c r="D108" s="82">
         <v>2.5550000000000002</v>
       </c>
-      <c r="E108" s="91">
+      <c r="E108" s="85">
         <v>121.3</v>
       </c>
-      <c r="F108" s="94">
+      <c r="F108" s="88">
         <v>60</v>
       </c>
       <c r="G108" s="8">
@@ -3421,16 +3421,16 @@
       <c r="B109" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C109" s="84" t="s">
+      <c r="C109" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D109" s="87">
+      <c r="D109" s="81">
         <v>0.19500000000000001</v>
       </c>
-      <c r="E109" s="90">
+      <c r="E109" s="84">
         <v>15.68</v>
       </c>
-      <c r="F109" s="93">
+      <c r="F109" s="87">
         <v>99</v>
       </c>
       <c r="G109" s="11">
@@ -3441,16 +3441,16 @@
       <c r="B110" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C110" s="83" t="s">
+      <c r="C110" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D110" s="88">
+      <c r="D110" s="82">
         <v>180</v>
       </c>
-      <c r="E110" s="91">
+      <c r="E110" s="85">
         <v>1317.82</v>
       </c>
-      <c r="F110" s="94" t="s">
+      <c r="F110" s="88" t="s">
         <v>14</v>
       </c>
       <c r="G110" s="8">
@@ -3461,16 +3461,16 @@
       <c r="B111" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C111" s="84" t="s">
+      <c r="C111" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D111" s="87">
+      <c r="D111" s="81">
         <v>8.0129999999999999</v>
       </c>
-      <c r="E111" s="90">
+      <c r="E111" s="84">
         <v>554.48</v>
       </c>
-      <c r="F111" s="93">
+      <c r="F111" s="87">
         <v>140</v>
       </c>
       <c r="G111" s="11">
@@ -3478,113 +3478,113 @@
       </c>
     </row>
     <row r="112" spans="2:7">
-      <c r="B112" s="98" t="s">
+      <c r="B112" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="C112" s="99" t="s">
+      <c r="C112" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="D112" s="100">
+      <c r="D112" s="94">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="E112" s="101">
+      <c r="E112" s="95">
         <v>4.84</v>
       </c>
-      <c r="F112" s="102">
+      <c r="F112" s="96">
         <v>62</v>
       </c>
-      <c r="G112" s="103">
+      <c r="G112" s="97">
         <v>123</v>
       </c>
     </row>
     <row r="113" spans="2:7">
-      <c r="B113" s="98" t="s">
+      <c r="B113" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C113" s="99" t="s">
+      <c r="C113" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="D113" s="100">
+      <c r="D113" s="94">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E113" s="101">
+      <c r="E113" s="95">
         <v>10.84</v>
       </c>
-      <c r="F113" s="102">
+      <c r="F113" s="96">
         <v>62</v>
       </c>
-      <c r="G113" s="103">
+      <c r="G113" s="97">
         <v>309</v>
       </c>
     </row>
     <row r="114" spans="2:7" ht="20" thickBot="1">
-      <c r="B114" s="104" t="s">
+      <c r="B114" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="C114" s="105" t="s">
+      <c r="C114" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="D114" s="106">
+      <c r="D114" s="100">
         <v>172.18299999999999</v>
       </c>
-      <c r="E114" s="107">
+      <c r="E114" s="101">
         <v>8192</v>
       </c>
-      <c r="F114" s="108" t="s">
+      <c r="F114" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="G114" s="109">
+      <c r="G114" s="103">
         <v>813831</v>
       </c>
     </row>
     <row r="115" spans="2:7" ht="20" thickBot="1"/>
     <row r="116" spans="2:7">
-      <c r="B116" s="79" t="s">
+      <c r="B116" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="C116" s="80"/>
-      <c r="D116" s="80"/>
-      <c r="E116" s="80"/>
-      <c r="F116" s="80"/>
-      <c r="G116" s="81"/>
+      <c r="C116" s="105"/>
+      <c r="D116" s="105"/>
+      <c r="E116" s="105"/>
+      <c r="F116" s="105"/>
+      <c r="G116" s="106"/>
     </row>
     <row r="117" spans="2:7">
-      <c r="B117" s="82" t="s">
+      <c r="B117" s="76" t="s">
         <v>0</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D117" s="85" t="s">
+      <c r="D117" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="E117" s="85" t="s">
+      <c r="E117" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="F117" s="85" t="s">
+      <c r="F117" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="G117" s="95" t="s">
+      <c r="G117" s="89" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="118" spans="2:7">
-      <c r="B118" s="96" t="s">
+      <c r="B118" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="C118" s="83" t="s">
+      <c r="C118" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D118" s="86">
+      <c r="D118" s="80">
         <v>5.5E-2</v>
       </c>
-      <c r="E118" s="89">
+      <c r="E118" s="83">
         <v>3.65</v>
       </c>
-      <c r="F118" s="92">
+      <c r="F118" s="86">
         <v>19</v>
       </c>
-      <c r="G118" s="97">
+      <c r="G118" s="91">
         <v>75</v>
       </c>
     </row>
@@ -3592,16 +3592,16 @@
       <c r="B119" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C119" s="84" t="s">
+      <c r="C119" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D119" s="87">
+      <c r="D119" s="81">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E119" s="90">
+      <c r="E119" s="84">
         <v>3.65</v>
       </c>
-      <c r="F119" s="93">
+      <c r="F119" s="87">
         <v>21</v>
       </c>
       <c r="G119" s="11">
@@ -3612,16 +3612,16 @@
       <c r="B120" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C120" s="83" t="s">
+      <c r="C120" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D120" s="88">
+      <c r="D120" s="82">
         <v>0.11899999999999999</v>
       </c>
-      <c r="E120" s="91">
+      <c r="E120" s="85">
         <v>8.56</v>
       </c>
-      <c r="F120" s="94">
+      <c r="F120" s="88">
         <v>19</v>
       </c>
       <c r="G120" s="8">
@@ -3632,16 +3632,16 @@
       <c r="B121" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C121" s="84" t="s">
+      <c r="C121" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D121" s="87">
+      <c r="D121" s="81">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="E121" s="90">
+      <c r="E121" s="84">
         <v>3.65</v>
       </c>
-      <c r="F121" s="93">
+      <c r="F121" s="87">
         <v>21</v>
       </c>
       <c r="G121" s="11">
@@ -3652,16 +3652,16 @@
       <c r="B122" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C122" s="83" t="s">
+      <c r="C122" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D122" s="88">
+      <c r="D122" s="82">
         <v>1.35</v>
       </c>
-      <c r="E122" s="91">
+      <c r="E122" s="85">
         <v>37.270000000000003</v>
       </c>
-      <c r="F122" s="94">
+      <c r="F122" s="88">
         <v>8</v>
       </c>
       <c r="G122" s="8">
@@ -3672,16 +3672,16 @@
       <c r="B123" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C123" s="84" t="s">
+      <c r="C123" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D123" s="87">
+      <c r="D123" s="81">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E123" s="90">
+      <c r="E123" s="84">
         <v>3.72</v>
       </c>
-      <c r="F123" s="93">
+      <c r="F123" s="87">
         <v>8</v>
       </c>
       <c r="G123" s="11">
@@ -3692,16 +3692,16 @@
       <c r="B124" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C124" s="83" t="s">
+      <c r="C124" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D124" s="88">
+      <c r="D124" s="82">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="E124" s="91">
+      <c r="E124" s="85">
         <v>3.37</v>
       </c>
-      <c r="F124" s="94">
+      <c r="F124" s="88">
         <v>3</v>
       </c>
       <c r="G124" s="8">
@@ -3712,16 +3712,16 @@
       <c r="B125" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C125" s="84" t="s">
+      <c r="C125" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D125" s="87">
+      <c r="D125" s="81">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="E125" s="90">
+      <c r="E125" s="84">
         <v>3.37</v>
       </c>
-      <c r="F125" s="93">
+      <c r="F125" s="87">
         <v>3</v>
       </c>
       <c r="G125" s="11">
@@ -3732,16 +3732,16 @@
       <c r="B126" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C126" s="83" t="s">
+      <c r="C126" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D126" s="88">
+      <c r="D126" s="82">
         <v>5.1269999999999998</v>
       </c>
-      <c r="E126" s="91">
+      <c r="E126" s="85">
         <v>162.5</v>
       </c>
-      <c r="F126" s="94">
+      <c r="F126" s="88">
         <v>62</v>
       </c>
       <c r="G126" s="8">
@@ -3752,16 +3752,16 @@
       <c r="B127" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C127" s="84" t="s">
+      <c r="C127" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D127" s="87">
+      <c r="D127" s="81">
         <v>0.19500000000000001</v>
       </c>
-      <c r="E127" s="90">
+      <c r="E127" s="84">
         <v>15.68</v>
       </c>
-      <c r="F127" s="93">
+      <c r="F127" s="87">
         <v>99</v>
       </c>
       <c r="G127" s="11">
@@ -3772,16 +3772,16 @@
       <c r="B128" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C128" s="83" t="s">
+      <c r="C128" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D128" s="88">
+      <c r="D128" s="82">
         <v>180</v>
       </c>
-      <c r="E128" s="91">
+      <c r="E128" s="85">
         <v>1317.82</v>
       </c>
-      <c r="F128" s="94" t="s">
+      <c r="F128" s="88" t="s">
         <v>14</v>
       </c>
       <c r="G128" s="8">
@@ -3792,16 +3792,16 @@
       <c r="B129" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C129" s="84" t="s">
+      <c r="C129" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D129" s="87">
+      <c r="D129" s="81">
         <v>3.1920000000000002</v>
       </c>
-      <c r="E129" s="90">
+      <c r="E129" s="84">
         <v>62.35</v>
       </c>
-      <c r="F129" s="93">
+      <c r="F129" s="87">
         <v>240</v>
       </c>
       <c r="G129" s="11">
@@ -3809,62 +3809,62 @@
       </c>
     </row>
     <row r="130" spans="2:7">
-      <c r="B130" s="98" t="s">
+      <c r="B130" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="C130" s="99" t="s">
+      <c r="C130" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="D130" s="100">
+      <c r="D130" s="94">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="E130" s="101">
+      <c r="E130" s="95">
         <v>4</v>
       </c>
-      <c r="F130" s="102">
+      <c r="F130" s="96">
         <v>62</v>
       </c>
-      <c r="G130" s="103">
+      <c r="G130" s="97">
         <v>123</v>
       </c>
     </row>
     <row r="131" spans="2:7">
-      <c r="B131" s="98" t="s">
+      <c r="B131" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C131" s="99" t="s">
+      <c r="C131" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="D131" s="100">
+      <c r="D131" s="94">
         <v>0.27200000000000002</v>
       </c>
-      <c r="E131" s="101">
+      <c r="E131" s="95">
         <v>9.4</v>
       </c>
-      <c r="F131" s="102">
+      <c r="F131" s="96">
         <v>62</v>
       </c>
-      <c r="G131" s="103">
+      <c r="G131" s="97">
         <v>309</v>
       </c>
     </row>
     <row r="132" spans="2:7" ht="20" thickBot="1">
-      <c r="B132" s="104" t="s">
+      <c r="B132" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="C132" s="105" t="s">
+      <c r="C132" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="D132" s="106">
+      <c r="D132" s="100">
         <v>180</v>
       </c>
-      <c r="E132" s="107">
+      <c r="E132" s="101">
         <v>668.72</v>
       </c>
-      <c r="F132" s="108" t="s">
+      <c r="F132" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="G132" s="109">
+      <c r="G132" s="103">
         <v>59024</v>
       </c>
     </row>

</xml_diff>

<commit_message>
benchmarks excel file is up to date
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sejaldua/Desktop/DIS/AI/sejelo-searchclient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65B8791E-AE28-0745-874A-E9B3ABD8973F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84036D4D-BE37-8240-88F4-442B10E51569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13160" yWindow="460" windowWidth="14440" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
+    <workbookView xWindow="15740" yWindow="460" windowWidth="12680" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="52">
   <si>
     <t>Level</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Table 2: Heuristic Implementation #2 using best-first search client - Exercise 5</t>
+  </si>
+  <si>
+    <t>Table 2: Heuristic Implementation #3 using best-first search client - Exercise 5</t>
   </si>
 </sst>
 </file>
@@ -1427,10 +1430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7093C41-8786-554E-A962-A4525C17734E}">
-  <dimension ref="B1:H132"/>
+  <dimension ref="B1:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G133" sqref="G133"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="87" workbookViewId="0">
+      <selection activeCell="D151" sqref="D151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3868,8 +3871,340 @@
         <v>59024</v>
       </c>
     </row>
+    <row r="133" spans="2:7" ht="20" thickBot="1"/>
+    <row r="134" spans="2:7">
+      <c r="B134" s="104" t="s">
+        <v>51</v>
+      </c>
+      <c r="C134" s="105"/>
+      <c r="D134" s="105"/>
+      <c r="E134" s="105"/>
+      <c r="F134" s="105"/>
+      <c r="G134" s="106"/>
+    </row>
+    <row r="135" spans="2:7">
+      <c r="B135" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D135" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E135" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="F135" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="G135" s="89" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7">
+      <c r="B136" s="90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C136" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D136" s="80">
+        <v>0.128</v>
+      </c>
+      <c r="E136" s="83">
+        <v>3.65</v>
+      </c>
+      <c r="F136" s="86">
+        <v>19</v>
+      </c>
+      <c r="G136" s="91">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7">
+      <c r="B137" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C137" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D137" s="81">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="E137" s="84">
+        <v>3.65</v>
+      </c>
+      <c r="F137" s="87">
+        <v>21</v>
+      </c>
+      <c r="G137" s="11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7">
+      <c r="B138" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C138" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D138" s="82">
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="E138" s="85">
+        <v>57.85</v>
+      </c>
+      <c r="F138" s="88">
+        <v>19</v>
+      </c>
+      <c r="G138" s="8">
+        <v>19413</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7">
+      <c r="B139" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C139" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D139" s="81">
+        <v>0.755</v>
+      </c>
+      <c r="E139" s="84">
+        <v>53.25</v>
+      </c>
+      <c r="F139" s="87">
+        <v>21</v>
+      </c>
+      <c r="G139" s="11">
+        <v>4437</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7">
+      <c r="B140" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C140" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D140" s="82">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="E140" s="85">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="F140" s="88">
+        <v>8</v>
+      </c>
+      <c r="G140" s="8">
+        <v>3401</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7">
+      <c r="B141" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C141" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D141" s="81">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E141" s="84">
+        <v>4</v>
+      </c>
+      <c r="F141" s="87">
+        <v>10</v>
+      </c>
+      <c r="G141" s="11">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7">
+      <c r="B142" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D142" s="82">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E142" s="85">
+        <v>3.37</v>
+      </c>
+      <c r="F142" s="88">
+        <v>3</v>
+      </c>
+      <c r="G142" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7">
+      <c r="B143" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D143" s="81">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E143" s="84">
+        <v>3.37</v>
+      </c>
+      <c r="F143" s="87">
+        <v>3</v>
+      </c>
+      <c r="G143" s="11">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7">
+      <c r="B144" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D144" s="82">
+        <v>3.1259999999999999</v>
+      </c>
+      <c r="E144" s="85">
+        <v>73.23</v>
+      </c>
+      <c r="F144" s="88">
+        <v>72</v>
+      </c>
+      <c r="G144" s="8">
+        <v>39157</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7">
+      <c r="B145" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C145" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D145" s="81">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="E145" s="84">
+        <v>31.36</v>
+      </c>
+      <c r="F145" s="87">
+        <v>140</v>
+      </c>
+      <c r="G145" s="11">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="146" spans="2:7">
+      <c r="B146" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C146" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D146" s="82">
+        <v>180</v>
+      </c>
+      <c r="E146" s="85">
+        <v>1403.99</v>
+      </c>
+      <c r="F146" s="88" t="s">
+        <v>14</v>
+      </c>
+      <c r="G146" s="8">
+        <v>2285375</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7">
+      <c r="B147" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C147" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D147" s="81">
+        <v>14.836</v>
+      </c>
+      <c r="E147" s="84">
+        <v>169.72</v>
+      </c>
+      <c r="F147" s="87">
+        <v>190</v>
+      </c>
+      <c r="G147" s="11">
+        <v>202358</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7">
+      <c r="B148" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="C148" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="D148" s="94">
+        <v>0.126</v>
+      </c>
+      <c r="E148" s="95">
+        <v>4</v>
+      </c>
+      <c r="F148" s="96">
+        <v>62</v>
+      </c>
+      <c r="G148" s="97">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7">
+      <c r="B149" s="92" t="s">
+        <v>47</v>
+      </c>
+      <c r="C149" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="D149" s="94">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="E149" s="95">
+        <v>9.4</v>
+      </c>
+      <c r="F149" s="96">
+        <v>62</v>
+      </c>
+      <c r="G149" s="97">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" ht="20" thickBot="1">
+      <c r="B150" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="C150" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="D150" s="100">
+        <v>180</v>
+      </c>
+      <c r="E150" s="101">
+        <v>758.72</v>
+      </c>
+      <c r="F150" s="102" t="s">
+        <v>14</v>
+      </c>
+      <c r="G150" s="103">
+        <v>59024</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B134:G134"/>
     <mergeCell ref="B98:G98"/>
     <mergeCell ref="B116:G116"/>
     <mergeCell ref="B80:G80"/>

</xml_diff>

<commit_message>
pushing downloaded report-- things are good to go if we don't have time to change stuff
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sejaldua/Desktop/DIS/AI/sejelo-searchclient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84036D4D-BE37-8240-88F4-442B10E51569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DCF07E-35B8-E242-B748-0A2C0154E397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15740" yWindow="460" windowWidth="12680" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
+    <workbookView xWindow="520" yWindow="460" windowWidth="16860" windowHeight="16800" xr2:uid="{F6752587-1176-1A44-BECD-10FAEDCF4C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="53">
   <si>
     <t>Level</t>
   </si>
@@ -186,7 +186,10 @@
     <t>Table 2: Heuristic Implementation #2 using best-first search client - Exercise 5</t>
   </si>
   <si>
-    <t>Table 2: Heuristic Implementation #3 using best-first search client - Exercise 5</t>
+    <t>Table 3: Heuristic Implementation #3 using best-first search client - Exercise 5</t>
+  </si>
+  <si>
+    <t>Table 4: Heuristic Implementation #4 using best-first search client - Exercise 5</t>
   </si>
 </sst>
 </file>
@@ -1430,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7093C41-8786-554E-A962-A4525C17734E}">
-  <dimension ref="B1:H150"/>
+  <dimension ref="B1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D151" sqref="D151"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="J167" sqref="J167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3719,7 +3722,7 @@
         <v>45</v>
       </c>
       <c r="D125" s="81">
-        <v>5.7000000000000002E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="E125" s="84">
         <v>3.37</v>
@@ -3759,16 +3762,16 @@
         <v>45</v>
       </c>
       <c r="D127" s="81">
-        <v>0.19500000000000001</v>
+        <v>3.1920000000000002</v>
       </c>
       <c r="E127" s="84">
-        <v>15.68</v>
+        <v>62.35</v>
       </c>
       <c r="F127" s="87">
-        <v>99</v>
+        <v>240</v>
       </c>
       <c r="G127" s="11">
-        <v>787</v>
+        <v>19353</v>
       </c>
     </row>
     <row r="128" spans="2:7">
@@ -3782,13 +3785,13 @@
         <v>180</v>
       </c>
       <c r="E128" s="85">
-        <v>1317.82</v>
+        <v>1942.99</v>
       </c>
       <c r="F128" s="88" t="s">
         <v>14</v>
       </c>
       <c r="G128" s="8">
-        <v>1888924</v>
+        <v>2484912</v>
       </c>
     </row>
     <row r="129" spans="2:7">
@@ -3799,16 +3802,16 @@
         <v>45</v>
       </c>
       <c r="D129" s="81">
-        <v>3.1920000000000002</v>
+        <v>25.474</v>
       </c>
       <c r="E129" s="84">
-        <v>62.35</v>
+        <v>1546.53</v>
       </c>
       <c r="F129" s="87">
-        <v>240</v>
+        <v>334</v>
       </c>
       <c r="G129" s="11">
-        <v>19353</v>
+        <v>510164</v>
       </c>
     </row>
     <row r="130" spans="2:7">
@@ -4202,9 +4205,341 @@
         <v>59024</v>
       </c>
     </row>
+    <row r="151" spans="2:7" ht="20" thickBot="1"/>
+    <row r="152" spans="2:7">
+      <c r="B152" s="104" t="s">
+        <v>52</v>
+      </c>
+      <c r="C152" s="105"/>
+      <c r="D152" s="105"/>
+      <c r="E152" s="105"/>
+      <c r="F152" s="105"/>
+      <c r="G152" s="106"/>
+    </row>
+    <row r="153" spans="2:7">
+      <c r="B153" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D153" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E153" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="F153" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="G153" s="89" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7">
+      <c r="B154" s="90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C154" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D154" s="80">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="E154" s="83">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="F154" s="86">
+        <v>19</v>
+      </c>
+      <c r="G154" s="91">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7">
+      <c r="B155" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C155" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D155" s="81">
+        <v>0.124</v>
+      </c>
+      <c r="E155" s="84">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="F155" s="87">
+        <v>19</v>
+      </c>
+      <c r="G155" s="11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="156" spans="2:7">
+      <c r="B156" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D156" s="82">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="E156" s="85">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="F156" s="88">
+        <v>19</v>
+      </c>
+      <c r="G156" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="157" spans="2:7">
+      <c r="B157" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D157" s="81">
+        <v>0.11</v>
+      </c>
+      <c r="E157" s="84">
+        <v>4.18</v>
+      </c>
+      <c r="F157" s="87">
+        <v>19</v>
+      </c>
+      <c r="G157" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7">
+      <c r="B158" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C158" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D158" s="82">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="E158" s="85">
+        <v>13.15</v>
+      </c>
+      <c r="F158" s="88">
+        <v>8</v>
+      </c>
+      <c r="G158" s="8">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7">
+      <c r="B159" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C159" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D159" s="81">
+        <v>0.06</v>
+      </c>
+      <c r="E159" s="84">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="F159" s="87">
+        <v>8</v>
+      </c>
+      <c r="G159" s="11">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="160" spans="2:7">
+      <c r="B160" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C160" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D160" s="82">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E160" s="85">
+        <v>8</v>
+      </c>
+      <c r="F160" s="88">
+        <v>3</v>
+      </c>
+      <c r="G160" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7">
+      <c r="B161" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C161" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D161" s="81">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="E161" s="84">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="F161" s="87">
+        <v>3</v>
+      </c>
+      <c r="G161" s="11">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7">
+      <c r="B162" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C162" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D162" s="82">
+        <v>1.9590000000000001</v>
+      </c>
+      <c r="E162" s="85">
+        <v>193.39</v>
+      </c>
+      <c r="F162" s="88">
+        <v>62</v>
+      </c>
+      <c r="G162" s="8">
+        <v>29629</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7">
+      <c r="B163" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C163" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D163" s="81">
+        <v>1.361</v>
+      </c>
+      <c r="E163" s="84">
+        <v>80.13</v>
+      </c>
+      <c r="F163" s="87">
+        <v>206</v>
+      </c>
+      <c r="G163" s="11">
+        <v>15218</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7">
+      <c r="B164" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C164" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D164" s="82">
+        <v>180</v>
+      </c>
+      <c r="E164" s="85">
+        <v>1929.75</v>
+      </c>
+      <c r="F164" s="88" t="s">
+        <v>14</v>
+      </c>
+      <c r="G164" s="8">
+        <v>2916068</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7">
+      <c r="B165" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C165" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D165" s="81">
+        <v>1.891</v>
+      </c>
+      <c r="E165" s="84">
+        <v>201.1</v>
+      </c>
+      <c r="F165" s="87">
+        <v>147</v>
+      </c>
+      <c r="G165" s="11">
+        <v>37380</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7">
+      <c r="B166" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="C166" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="D166" s="94">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="E166" s="95">
+        <v>5.37</v>
+      </c>
+      <c r="F166" s="96">
+        <v>62</v>
+      </c>
+      <c r="G166" s="97">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="167" spans="2:7">
+      <c r="B167" s="92" t="s">
+        <v>47</v>
+      </c>
+      <c r="C167" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="D167" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="E167" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="F167" s="96" t="s">
+        <v>14</v>
+      </c>
+      <c r="G167" s="97" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7" ht="20" thickBot="1">
+      <c r="B168" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="C168" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="D168" s="100" t="s">
+        <v>14</v>
+      </c>
+      <c r="E168" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="F168" s="102" t="s">
+        <v>14</v>
+      </c>
+      <c r="G168" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="B134:G134"/>
+    <mergeCell ref="B152:G152"/>
     <mergeCell ref="B98:G98"/>
     <mergeCell ref="B116:G116"/>
     <mergeCell ref="B80:G80"/>

</xml_diff>